<commit_message>
Hero/Henchmen equi cost fixed and 5 extra point added to the warband rating.
</commit_message>
<xml_diff>
--- a/kai/kai-warband_orks_mostlyepic_goblins.xlsx
+++ b/kai/kai-warband_orks_mostlyepic_goblins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\Dropbox\Privat\Mordheim\kai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{359AB0E1-D11F-48CF-9D45-809BCF922B24}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{71DD095A-6B66-464C-A0BA-679F6B6B501B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Member" sheetId="1" r:id="rId1"/>
@@ -887,8 +887,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C24:U42" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="C24:U42" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="C21:U39" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ausrüstung gesamt"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Typ"/>
@@ -1207,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AD123"/>
+  <dimension ref="A2:AD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O40" sqref="I40:O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1280,8 +1280,8 @@
         <v>73</v>
       </c>
       <c r="I4" s="10">
-        <f>5*SUM(E14:E20)+E14*F14+E15*F15+E16*F16+E17*F17+E18*F18+E19*F19+E20*F20</f>
-        <v>115</v>
+        <f>5*SUM(E11:E17)+E11*F11+E12*F12+E13*F13+E14*F14+E15*F15+E16*F16+E17*F17+5</f>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>137</v>
       </c>
       <c r="I5" s="10">
-        <f>E21/4</f>
+        <f>E18/4</f>
         <v>2</v>
       </c>
     </row>
@@ -1304,22 +1304,22 @@
         <v>18</v>
       </c>
       <c r="C6" s="4">
-        <f>G21+P43</f>
+        <f>G18+P40</f>
         <v>500</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>142</v>
       </c>
       <c r="I6" s="38">
-        <f>U43</f>
+        <f>U40</f>
         <v>145</v>
       </c>
       <c r="J6" s="6">
-        <f>U44</f>
+        <f>U41</f>
         <v>71</v>
       </c>
       <c r="K6" s="6">
-        <f>U45</f>
+        <f>U42</f>
         <v>74</v>
       </c>
     </row>
@@ -1333,313 +1333,489 @@
       </c>
       <c r="I7" s="2">
         <f>I3+(I6+I4)*I5</f>
-        <v>530</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="6">
+        <v>80</v>
+      </c>
+      <c r="E11" s="27">
+        <v>1</v>
+      </c>
+      <c r="F11" s="27">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G17" si="0">E11*D11</f>
+        <v>80</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="39"/>
+      <c r="C12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="6">
+        <v>40</v>
+      </c>
+      <c r="E12" s="27">
+        <v>1</v>
+      </c>
+      <c r="F12" s="27">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
       <c r="Q12" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="C13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>144</v>
+      <c r="B13" s="39"/>
+      <c r="C13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="6">
+        <v>40</v>
+      </c>
+      <c r="E13" s="27">
+        <v>3</v>
+      </c>
+      <c r="F13" s="27">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="39" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D14" s="6">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="E14" s="27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F14" s="27">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G20" si="0">E14*D14</f>
-        <v>80</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>145</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="39"/>
       <c r="C15" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D15" s="6">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E15" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="27">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="39"/>
       <c r="C16" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D16" s="6">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E16" s="27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16" s="27">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="39"/>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5">
+        <v>200</v>
+      </c>
+      <c r="E17" s="28">
+        <v>0</v>
+      </c>
+      <c r="F17" s="28">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="2">
+        <f>SUM(E11:E17)</f>
+        <v>8</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="2">
+        <f>SUM(G11:G17)</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+      <c r="F19" s="1"/>
+      <c r="I19" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+    </row>
+    <row r="20" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="I20" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="T20" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21"/>
+      <c r="C21" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="R21" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T21" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="U21" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22"/>
+      <c r="C22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="29"/>
+      <c r="G22" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="6">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6">
+        <v>0</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>0</v>
+      </c>
+      <c r="R22" s="6">
+        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="T22" s="30">
+        <v>1</v>
+      </c>
+      <c r="U22" s="30">
+        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23"/>
+      <c r="C23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="29"/>
+      <c r="G23" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="6">
+        <v>5</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+      <c r="K23" s="6">
+        <v>2</v>
+      </c>
+      <c r="L23" s="6">
+        <v>0</v>
+      </c>
+      <c r="M23" s="6">
+        <v>0</v>
+      </c>
+      <c r="N23" s="6">
+        <v>0</v>
+      </c>
+      <c r="O23" s="6">
+        <v>0</v>
+      </c>
+      <c r="P23" s="6">
+        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
         <v>15</v>
       </c>
-      <c r="E17" s="27">
-        <v>3</v>
-      </c>
-      <c r="F17" s="27">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B18" s="39"/>
-      <c r="C18" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="6">
-        <v>15</v>
-      </c>
-      <c r="E18" s="27">
-        <v>0</v>
-      </c>
-      <c r="F18" s="27">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B19" s="39"/>
-      <c r="C19" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="6">
-        <v>25</v>
-      </c>
-      <c r="E19" s="27">
-        <v>0</v>
-      </c>
-      <c r="F19" s="27">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="5">
-        <v>200</v>
-      </c>
-      <c r="E20" s="28">
-        <v>0</v>
-      </c>
-      <c r="F20" s="28">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="2">
-        <f>SUM(E14:E20)</f>
-        <v>8</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="2">
-        <f>SUM(G14:G20)</f>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="17"/>
-      <c r="F22" s="1"/>
-      <c r="I22" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-    </row>
-    <row r="23" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="I23" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-      <c r="T23" s="6" t="s">
-        <v>139</v>
+      <c r="Q23" s="6">
+        <v>0</v>
+      </c>
+      <c r="R23" s="6">
+        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="T23" s="30">
+        <v>4</v>
+      </c>
+      <c r="U23" s="30">
+        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24"/>
-      <c r="C24" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="M24" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="N24" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="O24" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="P24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q24" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="R24" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="S24" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="T24" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="U24" s="12" t="s">
-        <v>141</v>
+      <c r="C24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="6">
+        <v>15</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6">
+        <v>0</v>
+      </c>
+      <c r="M24" s="6">
+        <v>0</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>0</v>
+      </c>
+      <c r="R24" s="6">
+        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <v>0</v>
+      </c>
+      <c r="S24" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="T24" s="30">
+        <v>9</v>
+      </c>
+      <c r="U24" s="30">
+        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25"/>
       <c r="C25" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="18" t="s">
-        <v>102</v>
+      <c r="F25" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="H25" s="6">
+        <v>10</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0</v>
+      </c>
+      <c r="K25" s="6">
         <v>2</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" s="6">
-        <v>0</v>
-      </c>
-      <c r="K25" s="6">
-        <v>0</v>
-      </c>
       <c r="L25" s="6">
         <v>0</v>
       </c>
@@ -1652,9 +1828,9 @@
       <c r="O25" s="6">
         <v>0</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q25" s="6">
         <v>0</v>
@@ -1667,36 +1843,38 @@
         <v>128</v>
       </c>
       <c r="T25" s="30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U25" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26"/>
       <c r="C26" s="6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="29"/>
+      <c r="F26" s="29" t="s">
+        <v>108</v>
+      </c>
       <c r="G26" s="6" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="H26" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I26" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="6">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6">
         <v>1</v>
-      </c>
-      <c r="K26" s="6">
-        <v>2</v>
       </c>
       <c r="L26" s="6">
         <v>0</v>
@@ -1712,7 +1890,7 @@
       </c>
       <c r="P26" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -1725,29 +1903,29 @@
         <v>127</v>
       </c>
       <c r="T26" s="30">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U26" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27"/>
       <c r="C27" s="6" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>66</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H27" s="6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I27" s="6">
         <v>0</v>
@@ -1785,7 +1963,7 @@
         <v>127</v>
       </c>
       <c r="T27" s="30">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="U27" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
@@ -1795,19 +1973,14 @@
     <row r="28" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28"/>
       <c r="C28" s="6" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>107</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F28" s="29"/>
       <c r="H28" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I28" s="6">
         <v>0</v>
@@ -1816,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L28" s="6">
         <v>0</v>
@@ -1832,7 +2005,7 @@
       </c>
       <c r="P28" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="6">
         <v>0</v>
@@ -1845,38 +2018,41 @@
         <v>128</v>
       </c>
       <c r="T28" s="30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="U28" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29"/>
       <c r="C29" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>108</v>
+        <v>68</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="29">
+        <v>4</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="H29" s="6">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I29" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="6">
         <v>0</v>
       </c>
       <c r="K29" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="6">
         <v>0</v>
@@ -1892,7 +2068,7 @@
       </c>
       <c r="P29" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="6">
         <v>0</v>
@@ -1905,26 +2081,26 @@
         <v>127</v>
       </c>
       <c r="T29" s="30">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="U29" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30"/>
       <c r="C30" s="6" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>112</v>
+        <v>68</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="29">
+        <v>3</v>
       </c>
       <c r="H30" s="6">
         <v>10</v>
@@ -1936,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L30" s="6">
         <v>0</v>
@@ -1952,7 +2128,7 @@
       </c>
       <c r="P30" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Q30" s="6">
         <v>0</v>
@@ -1965,24 +2141,23 @@
         <v>127</v>
       </c>
       <c r="T30" s="30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U30" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B31"/>
       <c r="C31" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F31" s="29"/>
       <c r="H31" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I31" s="6">
         <v>0</v>
@@ -2017,10 +2192,10 @@
         <v>0</v>
       </c>
       <c r="S31" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T31" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U31" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
@@ -2028,24 +2203,20 @@
       </c>
     </row>
     <row r="32" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32"/>
       <c r="C32" s="6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="29">
-        <v>4</v>
+        <v>66</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H32" s="6">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I32" s="6">
         <v>0</v>
@@ -2057,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M32" s="6">
         <v>0</v>
@@ -2070,7 +2241,7 @@
       </c>
       <c r="P32" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q32" s="6">
         <v>0</v>
@@ -2080,32 +2251,31 @@
         <v>0</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T32" s="30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U32" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B33"/>
       <c r="C33" s="6" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>68</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="F33" s="29">
         <v>3</v>
       </c>
       <c r="H33" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I33" s="6">
         <v>0</v>
@@ -2114,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L33" s="6">
         <v>0</v>
@@ -2130,7 +2300,7 @@
       </c>
       <c r="P33" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="6">
         <v>0</v>
@@ -2140,26 +2310,29 @@
         <v>0</v>
       </c>
       <c r="S33" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T33" s="30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U33" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C34" s="6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>66</v>
+        <v>53</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>120</v>
       </c>
       <c r="F34" s="29"/>
       <c r="H34" s="6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I34" s="6">
         <v>0</v>
@@ -2206,19 +2379,19 @@
     </row>
     <row r="35" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C35" s="6" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>66</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H35" s="6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I35" s="6">
         <v>0</v>
@@ -2230,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="L35" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M35" s="6">
         <v>0</v>
@@ -2243,7 +2416,7 @@
       </c>
       <c r="P35" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="6">
         <v>0</v>
@@ -2256,28 +2429,25 @@
         <v>126</v>
       </c>
       <c r="T35" s="30">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="U35" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="29">
-        <v>3</v>
-      </c>
-      <c r="H36" s="6">
-        <v>5</v>
+      <c r="C36" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34">
+        <v>25</v>
       </c>
       <c r="I36" s="6">
         <v>0</v>
@@ -2324,26 +2494,26 @@
     </row>
     <row r="37" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C37" s="6" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="F37" s="29"/>
+      <c r="G37" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="H37" s="6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I37" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="6">
         <v>0</v>
       </c>
       <c r="K37" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L37" s="6">
         <v>0</v>
@@ -2359,7 +2529,7 @@
       </c>
       <c r="P37" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="Q37" s="6">
         <v>0</v>
@@ -2369,43 +2539,42 @@
         <v>0</v>
       </c>
       <c r="S37" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T37" s="30">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="U37" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C38" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F38" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>122</v>
+        <v>8</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="34"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="34" t="s">
+        <v>136</v>
       </c>
       <c r="H38" s="6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I38" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="6">
         <v>0</v>
       </c>
       <c r="K38" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M38" s="6">
         <v>0</v>
@@ -2418,7 +2587,7 @@
       </c>
       <c r="P38" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Q38" s="6">
         <v>0</v>
@@ -2428,31 +2597,31 @@
         <v>0</v>
       </c>
       <c r="S38" s="30" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="T38" s="30">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="U38" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C39" s="34" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E39" s="34"/>
       <c r="F39" s="35"/>
       <c r="G39" s="34"/>
       <c r="H39" s="34">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="6">
         <v>0</v>
@@ -2474,7 +2643,7 @@
       </c>
       <c r="P39" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q39" s="6">
         <v>0</v>
@@ -2484,333 +2653,165 @@
         <v>0</v>
       </c>
       <c r="S39" s="30" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="T39" s="30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U39" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F40" s="29"/>
-      <c r="G40" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H40" s="6">
-        <v>20</v>
-      </c>
-      <c r="I40" s="6">
-        <v>1</v>
-      </c>
-      <c r="J40" s="6">
-        <v>0</v>
-      </c>
-      <c r="K40" s="6">
-        <v>3</v>
-      </c>
-      <c r="L40" s="6">
-        <v>0</v>
-      </c>
-      <c r="M40" s="6">
-        <v>0</v>
-      </c>
-      <c r="N40" s="6">
-        <v>0</v>
-      </c>
-      <c r="O40" s="6">
-        <v>0</v>
-      </c>
-      <c r="P40" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>80</v>
-      </c>
-      <c r="Q40" s="6">
-        <v>0</v>
-      </c>
-      <c r="R40" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
-        <v>0</v>
-      </c>
-      <c r="S40" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="T40" s="30">
-        <v>8</v>
-      </c>
-      <c r="U40" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>32</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="3">
+        <f>I22*$H22+I23*$H23+I24*$H24+I25*$H25+I26*$H26+I27*$H27+I28*$H28+I29*$H29+I30*$H30+I31*$H31+I32*$H32+I33*$H33+I34*$H34+I35*$H35+I36*$H36+I37*$H37+I38*$H38+I39*$H39</f>
+        <v>45</v>
+      </c>
+      <c r="J40" s="3">
+        <f>J22*$H22+J23*$H23+J24*$H24+J25*$H25+J26*$H26+J27*$H27+J28*$H28+J29*$H29+J30*$H30+J31*$H31+J32*$H32+J33*$H33+J34*$H34+J35*$H35+J36*$H36+J37*$H37+J38*$H38+J39*$H39</f>
+        <v>5</v>
+      </c>
+      <c r="K40" s="3">
+        <f>K22*$H22+K23*$H23+K24*$H24+K25*$H25+K26*$H26+K27*$H27+K28*$H28+K29*$H29+K30*$H30+K31*$H31+K32*$H32+K33*$H33+K34*$H34+K35*$H35+K36*$H36+K37*$H37+K38*$H38+K39*$H39</f>
+        <v>135</v>
+      </c>
+      <c r="L40" s="3">
+        <f t="shared" ref="L40:O40" si="1">L22*$H22+L23*$H23+L24*$H24+L25*$H25+L26*$H26+L27*$H27+L28*$H28+L29*$H29+L30*$H30+L31*$H31+L32*$H32+L33*$H33+L34*$H34+L35*$H35+L36*$H36+L37*$H37+L38*$H38+L39*$H39</f>
+        <v>30</v>
+      </c>
+      <c r="M40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="2">
+        <f>SUM(P22:P39)</f>
+        <v>215</v>
+      </c>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="37">
+        <f>SUM(Tabelle2[zusatzkosten])</f>
+        <v>0</v>
+      </c>
+      <c r="S40" s="36"/>
+      <c r="T40" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="U40" s="2">
+        <f>SUM(Tabelle2[Warband Equip Rating])</f>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="34"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="H41" s="6">
-        <v>5</v>
-      </c>
-      <c r="I41" s="6">
-        <v>1</v>
-      </c>
-      <c r="J41" s="6">
-        <v>0</v>
-      </c>
-      <c r="K41" s="6">
-        <v>1</v>
-      </c>
-      <c r="L41" s="6">
-        <v>3</v>
-      </c>
-      <c r="M41" s="6">
-        <v>0</v>
-      </c>
-      <c r="N41" s="6">
-        <v>0</v>
-      </c>
-      <c r="O41" s="6">
-        <v>0</v>
-      </c>
-      <c r="P41" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>25</v>
-      </c>
-      <c r="Q41" s="6">
-        <v>0</v>
-      </c>
-      <c r="R41" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
-        <v>0</v>
-      </c>
-      <c r="S41" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="T41" s="30">
-        <v>7</v>
-      </c>
-      <c r="U41" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>35</v>
+      <c r="F41" s="29"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="U41" s="6">
+        <f>SUM(U22:U36)</f>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34">
-        <v>10</v>
-      </c>
-      <c r="I42" s="6">
-        <v>1</v>
-      </c>
-      <c r="J42" s="6">
-        <v>0</v>
-      </c>
-      <c r="K42" s="6">
-        <v>0</v>
-      </c>
-      <c r="L42" s="6">
-        <v>0</v>
-      </c>
-      <c r="M42" s="6">
-        <v>0</v>
-      </c>
-      <c r="N42" s="6">
-        <v>0</v>
-      </c>
-      <c r="O42" s="6">
-        <v>0</v>
-      </c>
-      <c r="P42" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>10</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>0</v>
-      </c>
-      <c r="R42" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
-        <v>0</v>
-      </c>
-      <c r="S42" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="T42" s="30">
-        <v>7</v>
-      </c>
-      <c r="U42" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43"/>
+      <c r="F42" s="29"/>
+      <c r="S42" s="30"/>
+      <c r="T42" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="U42" s="6">
+        <f>SUM(U37:U39)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
       <c r="F43" s="35"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="3">
-        <f>I25*$H25+I26*$H26+I27*$H27+I28*$H28+I29*$H29+I30*$H30+I31*$H31+I32*$H32+I33*$H33+I34*$H34+I35*$H35+I36*$H36+I37*$H37+I38*$H38+I39*H39+I40*H40+I41*H41+I42*H42</f>
-        <v>45</v>
-      </c>
-      <c r="J43" s="3">
-        <f t="shared" ref="J43:O43" si="1">J25*$H25+J26*$H26+J27*$H27+J28*$H28+J29*$H29+J30*$H30+J31*$H31+J32*$H32+J33*$H33+J34*$H34+J35*$H35+J36*$H36+J37*$H37+J38*$H38+J39*I39+J40*I40+J41*I41+J42*I42</f>
-        <v>5</v>
-      </c>
-      <c r="K43" s="3">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="L43" s="3">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="M43" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N43" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O43" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P43" s="2">
-        <f>SUM(P25:P42)</f>
-        <v>215</v>
-      </c>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="34"/>
+      <c r="P43" s="34"/>
       <c r="Q43" s="34"/>
-      <c r="R43" s="37">
-        <f>SUM(Tabelle2[zusatzkosten])</f>
-        <v>0</v>
-      </c>
+      <c r="R43" s="34"/>
       <c r="S43" s="36"/>
-      <c r="T43" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="U43" s="2">
-        <f>SUM(Tabelle2[Warband Equip Rating])</f>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="44" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F44" s="29"/>
-      <c r="S44" s="30"/>
-      <c r="T44" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="U44" s="6">
-        <f>SUM(U25:U39)</f>
-        <v>71</v>
-      </c>
+    </row>
+    <row r="44" spans="2:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C44"/>
+      <c r="H44"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="2"/>
     </row>
     <row r="45" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F45" s="29"/>
-      <c r="S45" s="30"/>
-      <c r="T45" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="U45" s="6">
-        <f>SUM(U40:U42)</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="34"/>
-      <c r="P46" s="34"/>
-      <c r="Q46" s="34"/>
-      <c r="R46" s="34"/>
-      <c r="S46" s="36"/>
-    </row>
-    <row r="47" spans="2:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47"/>
-      <c r="H47"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="2"/>
-    </row>
-    <row r="48" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G48"/>
-    </row>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="49" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="V55" s="1"/>
-    </row>
-    <row r="56" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="V56" s="1"/>
-    </row>
-    <row r="57" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-      <c r="P57" s="6"/>
-    </row>
-    <row r="58" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V52" s="1"/>
+    </row>
+    <row r="53" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V53" s="1"/>
+    </row>
+    <row r="54" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="P54" s="6"/>
+    </row>
+    <row r="55" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="P58"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+    </row>
     <row r="59" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="P61"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-    </row>
+    <row r="61" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2850,9 +2851,33 @@
     <row r="98" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="99" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="100" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="101" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="102" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="103" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="P101" s="6"/>
+    </row>
+    <row r="102" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="P102" s="6"/>
+    </row>
+    <row r="103" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="P103" s="6"/>
+    </row>
     <row r="104" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
@@ -2862,32 +2887,32 @@
       <c r="I104" s="6"/>
       <c r="P104" s="6"/>
     </row>
-    <row r="105" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="6"/>
-      <c r="P105" s="6"/>
-    </row>
-    <row r="106" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
-      <c r="H106" s="6"/>
-      <c r="I106" s="6"/>
-      <c r="P106" s="6"/>
-    </row>
-    <row r="107" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-      <c r="F107" s="6"/>
-      <c r="G107" s="6"/>
-      <c r="H107" s="6"/>
-      <c r="I107" s="6"/>
-      <c r="P107" s="6"/>
+    <row r="110" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C110"/>
+      <c r="D110"/>
+      <c r="F110"/>
+      <c r="G110"/>
+      <c r="H110"/>
+      <c r="I110"/>
+      <c r="P110"/>
+    </row>
+    <row r="111" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C111"/>
+      <c r="D111"/>
+      <c r="F111"/>
+      <c r="G111"/>
+      <c r="H111"/>
+      <c r="I111"/>
+      <c r="P111"/>
+    </row>
+    <row r="112" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C112"/>
+      <c r="D112"/>
+      <c r="F112"/>
+      <c r="G112"/>
+      <c r="H112"/>
+      <c r="I112"/>
+      <c r="P112"/>
     </row>
     <row r="113" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C113"/>
@@ -2898,37 +2923,37 @@
       <c r="I113"/>
       <c r="P113"/>
     </row>
-    <row r="114" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C114"/>
-      <c r="D114"/>
-      <c r="F114"/>
-      <c r="G114"/>
-      <c r="H114"/>
-      <c r="I114"/>
-      <c r="P114"/>
-    </row>
-    <row r="115" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C115"/>
-      <c r="D115"/>
-      <c r="F115"/>
-      <c r="G115"/>
-      <c r="H115"/>
-      <c r="I115"/>
-      <c r="P115"/>
-    </row>
-    <row r="116" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C116"/>
-      <c r="D116"/>
-      <c r="F116"/>
-      <c r="G116"/>
-      <c r="H116"/>
-      <c r="I116"/>
-      <c r="P116"/>
-    </row>
-    <row r="117" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="118" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="119" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="120" spans="3:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="115" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="116" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="117" spans="3:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="P117" s="6"/>
+    </row>
+    <row r="118" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="P118" s="6"/>
+    </row>
+    <row r="119" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="P119" s="6"/>
+    </row>
+    <row r="120" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="F120" s="6"/>
@@ -2937,47 +2962,20 @@
       <c r="I120" s="6"/>
       <c r="P120" s="6"/>
     </row>
-    <row r="121" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="6"/>
-      <c r="H121" s="6"/>
-      <c r="I121" s="6"/>
-      <c r="P121" s="6"/>
-    </row>
-    <row r="122" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="6"/>
-      <c r="H122" s="6"/>
-      <c r="I122" s="6"/>
-      <c r="P122" s="6"/>
-    </row>
-    <row r="123" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="F123" s="6"/>
-      <c r="G123" s="6"/>
-      <c r="H123" s="6"/>
-      <c r="I123" s="6"/>
-      <c r="P123" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="I22:O22"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="I19:O19"/>
   </mergeCells>
   <conditionalFormatting sqref="C6">
     <cfRule type="cellIs" dxfId="29" priority="55" operator="greaterThan">
       <formula>$C$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14:G20">
+  <conditionalFormatting sqref="G11:G17">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -2989,7 +2987,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P25:P42">
+  <conditionalFormatting sqref="P22:P39">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -3001,7 +2999,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D20">
+  <conditionalFormatting sqref="D11:D17">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3013,7 +3011,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43:H46">
+  <conditionalFormatting sqref="H40:H43">
     <cfRule type="colorScale" priority="134">
       <colorScale>
         <cfvo type="min"/>
@@ -3025,7 +3023,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P34:P42 P44:P46">
+  <conditionalFormatting sqref="P31:P39 P41:P43">
     <cfRule type="colorScale" priority="136">
       <colorScale>
         <cfvo type="min"/>
@@ -3037,7 +3035,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P44:P46 P25:P42">
+  <conditionalFormatting sqref="P41:P43 P22:P39">
     <cfRule type="colorScale" priority="138">
       <colorScale>
         <cfvo type="min"/>
@@ -3049,7 +3047,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:H33 H40:H42">
+  <conditionalFormatting sqref="H22:H30 H37:H39">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3061,7 +3059,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:H39">
+  <conditionalFormatting sqref="H31:H36">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3073,37 +3071,37 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
+  <conditionalFormatting sqref="I22">
     <cfRule type="cellIs" dxfId="28" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25:O25">
+  <conditionalFormatting sqref="J22:O22">
     <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26:I42">
+  <conditionalFormatting sqref="I23:I39">
     <cfRule type="cellIs" dxfId="26" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J26:O42">
+  <conditionalFormatting sqref="J23:O39">
     <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25:O42">
+  <conditionalFormatting sqref="I22:O39">
     <cfRule type="cellIs" dxfId="24" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E20">
+  <conditionalFormatting sqref="E11:E17">
     <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T25:T42">
+  <conditionalFormatting sqref="T22:T39">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3128,7 +3126,7 @@
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3167,31 +3165,31 @@
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="13"/>
       <c r="C4" s="12" t="str">
+        <f>Member!C11</f>
+        <v>ork boss (1)</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f>Member!C12</f>
+        <v>schamane (0-1)</v>
+      </c>
+      <c r="E4" s="12" t="str">
+        <f>Member!C13</f>
+        <v>big'uns (0-3)</v>
+      </c>
+      <c r="F4" s="12" t="str">
         <f>Member!C14</f>
-        <v>ork boss (1)</v>
-      </c>
-      <c r="D4" s="12" t="str">
+        <v>goblin warrior (max 2x anz boyz)</v>
+      </c>
+      <c r="G4" s="12" t="str">
         <f>Member!C15</f>
-        <v>schamane (0-1)</v>
-      </c>
-      <c r="E4" s="12" t="str">
+        <v>cave squig</v>
+      </c>
+      <c r="H4" s="12" t="str">
         <f>Member!C16</f>
-        <v>big'uns (0-3)</v>
-      </c>
-      <c r="F4" s="12" t="str">
+        <v>ork boy</v>
+      </c>
+      <c r="I4" s="12" t="str">
         <f>Member!C17</f>
-        <v>goblin warrior (max 2x anz boyz)</v>
-      </c>
-      <c r="G4" s="12" t="str">
-        <f>Member!C18</f>
-        <v>cave squig</v>
-      </c>
-      <c r="H4" s="12" t="str">
-        <f>Member!C19</f>
-        <v>ork boy</v>
-      </c>
-      <c r="I4" s="12" t="str">
-        <f>Member!C20</f>
         <v>troll</v>
       </c>
       <c r="K4" s="40" t="s">
@@ -3783,31 +3781,31 @@
         <v>46</v>
       </c>
       <c r="C24" s="11">
+        <f>Member!D11</f>
+        <v>80</v>
+      </c>
+      <c r="D24" s="11">
+        <f>Member!D12</f>
+        <v>40</v>
+      </c>
+      <c r="E24" s="11">
+        <f>Member!D13</f>
+        <v>40</v>
+      </c>
+      <c r="F24" s="11">
         <f>Member!D14</f>
-        <v>80</v>
-      </c>
-      <c r="D24" s="11">
+        <v>15</v>
+      </c>
+      <c r="G24" s="11">
         <f>Member!D15</f>
-        <v>40</v>
-      </c>
-      <c r="E24" s="11">
+        <v>15</v>
+      </c>
+      <c r="H24" s="11">
         <f>Member!D16</f>
-        <v>40</v>
-      </c>
-      <c r="F24" s="11">
+        <v>25</v>
+      </c>
+      <c r="I24" s="11">
         <f>Member!D17</f>
-        <v>15</v>
-      </c>
-      <c r="G24" s="11">
-        <f>Member!D18</f>
-        <v>15</v>
-      </c>
-      <c r="H24" s="11">
-        <f>Member!D19</f>
-        <v>25</v>
-      </c>
-      <c r="I24" s="11">
-        <f>Member!D20</f>
         <v>200</v>
       </c>
       <c r="J24" s="6"/>
@@ -3844,31 +3842,31 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C27">
-        <f>Member!$E14*'Characteristik analyse'!C26</f>
+        <f>Member!$E11*'Characteristik analyse'!C26</f>
         <v>2.0999999999999996</v>
       </c>
       <c r="D27" s="6">
-        <f>Member!$E15*'Characteristik analyse'!D26</f>
+        <f>Member!$E12*'Characteristik analyse'!D26</f>
         <v>3.4750000000000001</v>
       </c>
       <c r="E27" s="6">
-        <f>Member!$E16*'Characteristik analyse'!E26</f>
+        <f>Member!$E13*'Characteristik analyse'!E26</f>
         <v>11.175000000000001</v>
       </c>
       <c r="F27" s="6">
-        <f>Member!$E17*'Characteristik analyse'!F26</f>
+        <f>Member!$E14*'Characteristik analyse'!F26</f>
         <v>14.2</v>
       </c>
       <c r="G27" s="6">
-        <f>Member!$E18*'Characteristik analyse'!G26</f>
+        <f>Member!$E15*'Characteristik analyse'!G26</f>
         <v>0</v>
       </c>
       <c r="H27" s="6">
-        <f>Member!$E19*'Characteristik analyse'!H26</f>
+        <f>Member!$E16*'Characteristik analyse'!H26</f>
         <v>0</v>
       </c>
       <c r="I27" s="6">
-        <f>Member!$E20*'Characteristik analyse'!I26</f>
+        <f>Member!$E17*'Characteristik analyse'!I26</f>
         <v>0</v>
       </c>
       <c r="J27" s="1">
@@ -3939,8 +3937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4070,15 +4068,15 @@
         <v>3.15</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
-        <v>6.3</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="H7" s="32">
         <f>Tabelle4[[#This Row],[€ genutzt/Packung]]/Tabelle4[[#This Row],[€/Packung]]</f>
-        <v>0.66666666666666674</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
@@ -4354,7 +4352,7 @@
       </c>
       <c r="G18" s="9">
         <f>SUM(G4:G17)</f>
-        <v>18.934999999999999</v>
+        <v>22.084999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Warband detail list started.
</commit_message>
<xml_diff>
--- a/kai/kai-warband_orks_mostlyepic_goblins.xlsx
+++ b/kai/kai-warband_orks_mostlyepic_goblins.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\Dropbox\Privat\Mordheim\kai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{71DD095A-6B66-464C-A0BA-679F6B6B501B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{39F36BDB-D293-40D3-9BD7-315B3135AD3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Member" sheetId="1" r:id="rId1"/>
-    <sheet name="Characteristik analyse" sheetId="2" r:id="rId2"/>
-    <sheet name="Boxen" sheetId="4" r:id="rId3"/>
+    <sheet name="warband detail" sheetId="5" r:id="rId2"/>
+    <sheet name="Characteristik analyse" sheetId="2" r:id="rId3"/>
+    <sheet name="Boxen" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="164">
   <si>
     <t>gold</t>
   </si>
@@ -480,6 +481,45 @@
   </si>
   <si>
     <t>Magic rating</t>
+  </si>
+  <si>
+    <t>Big'Un 2</t>
+  </si>
+  <si>
+    <t>Big'Un 1</t>
+  </si>
+  <si>
+    <t>Big'Un 3</t>
+  </si>
+  <si>
+    <t>Axt</t>
+  </si>
+  <si>
+    <t>Schwert</t>
+  </si>
+  <si>
+    <t>Zweihänder</t>
+  </si>
+  <si>
+    <t>Speer</t>
+  </si>
+  <si>
+    <t>Schild</t>
+  </si>
+  <si>
+    <t>20xp</t>
+  </si>
+  <si>
+    <t>15xp</t>
+  </si>
+  <si>
+    <t>10xp</t>
+  </si>
+  <si>
+    <t>gc</t>
+  </si>
+  <si>
+    <t>Goblin Warrior</t>
   </si>
 </sst>
 </file>
@@ -490,7 +530,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -553,6 +593,23 @@
     </font>
     <font>
       <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -643,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -693,6 +750,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -702,11 +762,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -818,61 +934,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -887,36 +948,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="C21:U39" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ausrüstung gesamt"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Typ"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Range"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="S" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="S" dataDxfId="26"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SP"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="gold/stück"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Boss" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Boss" dataDxfId="25">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="schamane" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="big'uns" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="goblin" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="squig" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="boy" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="troll" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="kosten" dataDxfId="11">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="schamane" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="big'uns" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="goblin" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="squig" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="boy" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="troll" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="kosten" dataDxfId="18">
       <calculatedColumnFormula>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="wunsch" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="wunsch" dataDxfId="17">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="zusatzkosten" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="zusatzkosten" dataDxfId="16">
       <calculatedColumnFormula>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gruppe" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Bewertung" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Warband Equip Rating" dataDxfId="6">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gruppe" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Bewertung" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Warband Equip Rating" dataDxfId="13">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -925,18 +986,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle4" displayName="Tabelle4" ref="B3:H17" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle4" displayName="Tabelle4" ref="B3:H17" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="B3:H17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Mögliche einheiten" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="€/Packung" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Mögliche einheiten" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="€/Packung" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ausrüstung"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="€/Figur" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="€/Figur" dataDxfId="9"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Genutzte figuren"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="€ genutzt/Packung" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="€ genutzt/Packung" dataDxfId="8">
       <calculatedColumnFormula>F4*E4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Prozentuale Nutzung" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Prozentuale Nutzung" dataDxfId="7">
       <calculatedColumnFormula>Tabelle4[[#This Row],[€ genutzt/Packung]]/Tabelle4[[#This Row],[€/Packung]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1209,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD120"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O40" sqref="I40:O40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1352,7 @@
       <c r="C5" s="4">
         <v>500</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="6" t="s">
         <v>137</v>
       </c>
       <c r="I5" s="10">
@@ -1299,7 +1360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:18" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1323,7 +1384,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>15</v>
       </c>
@@ -1361,7 +1422,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="42" t="s">
         <v>95</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -1388,7 +1449,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="39"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="6" t="s">
         <v>97</v>
       </c>
@@ -1413,7 +1474,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="39"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="6" t="s">
         <v>98</v>
       </c>
@@ -1432,7 +1493,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="42" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1453,7 +1514,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="39"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="6" t="s">
         <v>100</v>
       </c>
@@ -1472,7 +1533,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="39"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="6" t="s">
         <v>101</v>
       </c>
@@ -1490,8 +1551,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="42"/>
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1509,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="16" t="s">
         <v>49</v>
       </c>
@@ -1526,36 +1587,35 @@
     <row r="19" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17"/>
       <c r="F19" s="1"/>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
     </row>
     <row r="20" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="I20" s="40" t="s">
+      <c r="I20" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40" t="s">
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
       <c r="T20" s="6" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="21" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21"/>
       <c r="C21" s="12" t="s">
         <v>90</v>
       </c>
@@ -1615,7 +1675,6 @@
       </c>
     </row>
     <row r="22" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22"/>
       <c r="C22" s="6" t="s">
         <v>9</v>
       </c>
@@ -1629,7 +1688,7 @@
       <c r="H22" s="6">
         <v>2</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="6">
         <v>0</v>
       </c>
       <c r="J22" s="6">
@@ -1650,7 +1709,7 @@
       <c r="O22" s="6">
         <v>0</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
         <v>0</v>
       </c>
@@ -1673,7 +1732,6 @@
       </c>
     </row>
     <row r="23" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23"/>
       <c r="C23" s="6" t="s">
         <v>1</v>
       </c>
@@ -1731,7 +1789,6 @@
       </c>
     </row>
     <row r="24" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24"/>
       <c r="C24" s="6" t="s">
         <v>104</v>
       </c>
@@ -1791,7 +1848,6 @@
       </c>
     </row>
     <row r="25" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B25"/>
       <c r="C25" s="6" t="s">
         <v>2</v>
       </c>
@@ -1851,7 +1907,6 @@
       </c>
     </row>
     <row r="26" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B26"/>
       <c r="C26" s="6" t="s">
         <v>3</v>
       </c>
@@ -1911,7 +1966,6 @@
       </c>
     </row>
     <row r="27" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27"/>
       <c r="C27" s="6" t="s">
         <v>110</v>
       </c>
@@ -1971,7 +2025,6 @@
       </c>
     </row>
     <row r="28" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B28"/>
       <c r="C28" s="6" t="s">
         <v>113</v>
       </c>
@@ -2026,7 +2079,6 @@
       </c>
     </row>
     <row r="29" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B29"/>
       <c r="C29" s="6" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2141,6 @@
       </c>
     </row>
     <row r="30" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30"/>
       <c r="C30" s="6" t="s">
         <v>5</v>
       </c>
@@ -2261,7 +2312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C33" s="6" t="s">
         <v>117</v>
       </c>
@@ -2320,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C34" s="6" t="s">
         <v>119</v>
       </c>
@@ -2377,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C35" s="6" t="s">
         <v>121</v>
       </c>
@@ -2436,7 +2487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C36" s="34" t="s">
         <v>123</v>
       </c>
@@ -2492,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C37" s="6" t="s">
         <v>6</v>
       </c>
@@ -2549,7 +2600,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C38" s="6" t="s">
         <v>8</v>
       </c>
@@ -2607,7 +2658,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C39" s="34" t="s">
         <v>7</v>
       </c>
@@ -2663,8 +2714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="2:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40"/>
+    <row r="40" spans="3:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
       <c r="E40" s="34"/>
@@ -2672,19 +2722,19 @@
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="3">
-        <f>I22*$H22+I23*$H23+I24*$H24+I25*$H25+I26*$H26+I27*$H27+I28*$H28+I29*$H29+I30*$H30+I31*$H31+I32*$H32+I33*$H33+I34*$H34+I35*$H35+I36*$H36+I37*$H37+I38*$H38+I39*$H39</f>
+        <f t="shared" ref="I40:O40" si="1">I22*$H22+I23*$H23+I24*$H24+I25*$H25+I26*$H26+I27*$H27+I28*$H28+I29*$H29+I30*$H30+I31*$H31+I32*$H32+I33*$H33+I34*$H34+I35*$H35+I36*$H36+I37*$H37+I38*$H38+I39*$H39</f>
         <v>45</v>
       </c>
       <c r="J40" s="3">
-        <f>J22*$H22+J23*$H23+J24*$H24+J25*$H25+J26*$H26+J27*$H27+J28*$H28+J29*$H29+J30*$H30+J31*$H31+J32*$H32+J33*$H33+J34*$H34+J35*$H35+J36*$H36+J37*$H37+J38*$H38+J39*$H39</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K40" s="3">
-        <f>K22*$H22+K23*$H23+K24*$H24+K25*$H25+K26*$H26+K27*$H27+K28*$H28+K29*$H29+K30*$H30+K31*$H31+K32*$H32+K33*$H33+K34*$H34+K35*$H35+K36*$H36+K37*$H37+K38*$H38+K39*$H39</f>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="L40" s="3">
-        <f t="shared" ref="L40:O40" si="1">L22*$H22+L23*$H23+L24*$H24+L25*$H25+L26*$H26+L27*$H27+L28*$H28+L29*$H29+L30*$H30+L31*$H31+L32*$H32+L33*$H33+L34*$H34+L35*$H35+L36*$H36+L37*$H37+L38*$H38+L39*$H39</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="M40" s="3">
@@ -2717,7 +2767,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F41" s="29"/>
       <c r="S41" s="30"/>
       <c r="T41" s="6" t="s">
@@ -2728,7 +2778,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F42" s="29"/>
       <c r="S42" s="30"/>
       <c r="T42" s="6" t="s">
@@ -2739,7 +2789,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
@@ -2758,24 +2808,17 @@
       <c r="R43" s="34"/>
       <c r="S43" s="36"/>
     </row>
-    <row r="44" spans="2:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C44"/>
-      <c r="H44"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
+    <row r="44" spans="3:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G45"/>
-    </row>
-    <row r="46" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="49" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2798,13 +2841,6 @@
     <row r="56" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C58"/>
-      <c r="D58"/>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-      <c r="P58"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
@@ -2887,42 +2923,10 @@
       <c r="I104" s="6"/>
       <c r="P104" s="6"/>
     </row>
-    <row r="110" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C110"/>
-      <c r="D110"/>
-      <c r="F110"/>
-      <c r="G110"/>
-      <c r="H110"/>
-      <c r="I110"/>
-      <c r="P110"/>
-    </row>
-    <row r="111" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C111"/>
-      <c r="D111"/>
-      <c r="F111"/>
-      <c r="G111"/>
-      <c r="H111"/>
-      <c r="I111"/>
-      <c r="P111"/>
-    </row>
-    <row r="112" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C112"/>
-      <c r="D112"/>
-      <c r="F112"/>
-      <c r="G112"/>
-      <c r="H112"/>
-      <c r="I112"/>
-      <c r="P112"/>
-    </row>
-    <row r="113" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C113"/>
-      <c r="D113"/>
-      <c r="F113"/>
-      <c r="G113"/>
-      <c r="H113"/>
-      <c r="I113"/>
-      <c r="P113"/>
-    </row>
+    <row r="110" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="112" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="113" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="114" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="115" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="116" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2966,12 +2970,12 @@
   <mergeCells count="5">
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B17"/>
+    <mergeCell ref="I19:O19"/>
     <mergeCell ref="I20:K20"/>
     <mergeCell ref="L20:O20"/>
-    <mergeCell ref="I19:O19"/>
   </mergeCells>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="29" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="55" operator="greaterThan">
       <formula>$C$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3072,32 +3076,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:O22">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I39">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:O39">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:O39">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E17">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3123,9 +3127,346 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:H42"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="39"/>
+      <c r="B3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="39">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3">
+        <f>C8+C16+C24+C32+C36+C42+C42+C42</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="39"/>
+      <c r="B6" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="39"/>
+      <c r="B7" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="40">
+        <f>SUM(C3:C7)</f>
+        <v>85</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="39"/>
+      <c r="B11" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="41">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="39"/>
+      <c r="B13" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="39"/>
+      <c r="B15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40">
+        <f>SUM(C11:C15)</f>
+        <v>85</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20">
+        <f>Member!H23</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21">
+        <f>Member!H25</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <f>Member!H30</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <f>Member!H37</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="3">
+        <f>SUM(C19:C23)</f>
+        <v>85</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28">
+        <f>Member!H26</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="3">
+        <f>SUM(C27:C31)</f>
+        <v>125</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="3">
+        <f>C35+C34</f>
+        <v>45</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="3">
+        <f>SUM(C39:C41)</f>
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -3150,17 +3491,17 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41" t="s">
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="13"/>
@@ -3192,10 +3533,10 @@
         <f>Member!C17</f>
         <v>troll</v>
       </c>
-      <c r="K4" s="40" t="s">
+      <c r="K4" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="40"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
@@ -3518,19 +3859,19 @@
         <v>1</v>
       </c>
       <c r="F15" s="31">
-        <f>$L6*F6/F$24</f>
-        <v>0.93333333333333335</v>
+        <f t="shared" ref="F15:I22" si="2">$L6*F6/F$24</f>
+        <v>0.93333333333330004</v>
       </c>
       <c r="G15" s="31">
-        <f>$L6*G6/G$24</f>
-        <v>1.8666666666666667</v>
+        <f t="shared" si="2"/>
+        <v>1.8666666666667</v>
       </c>
       <c r="H15" s="31">
-        <f>$L6*H6/H$24</f>
+        <f t="shared" si="2"/>
         <v>0.84</v>
       </c>
       <c r="I15" s="31">
-        <f>$L6*I6/I$24</f>
+        <f t="shared" si="2"/>
         <v>0.105</v>
       </c>
     </row>
@@ -3551,19 +3892,19 @@
         <v>0.75</v>
       </c>
       <c r="F16" s="31">
-        <f t="shared" ref="F16:F22" si="2">$L7*F7/F$24</f>
+        <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
       <c r="G16" s="31">
-        <f t="shared" ref="G16:I22" si="3">$L7*G7/G$24</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H16" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.84</v>
       </c>
       <c r="I16" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -3588,15 +3929,15 @@
         <v>1</v>
       </c>
       <c r="G17" s="31">
-        <f t="shared" si="3"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="2"/>
+        <v>1.3333333333333</v>
       </c>
       <c r="H17" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="I17" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
     </row>
@@ -3621,15 +3962,15 @@
         <v>1</v>
       </c>
       <c r="G18" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H18" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="I18" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
     </row>
@@ -3654,15 +3995,15 @@
         <v>0</v>
       </c>
       <c r="G19" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H19" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I19" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3687,15 +4028,15 @@
         <v>0.2</v>
       </c>
       <c r="G20" s="31">
-        <f t="shared" si="3"/>
-        <v>0.26666666666666666</v>
+        <f t="shared" si="2"/>
+        <v>0.26666666666670003</v>
       </c>
       <c r="H20" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.08</v>
       </c>
       <c r="I20" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -3717,18 +4058,18 @@
       </c>
       <c r="F21" s="31">
         <f t="shared" si="2"/>
-        <v>3.3333333333333333E-2</v>
+        <v>3.3333333333299998E-2</v>
       </c>
       <c r="G21" s="31">
-        <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.3333333333299998E-2</v>
       </c>
       <c r="H21" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="I21" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
@@ -3750,18 +4091,18 @@
       </c>
       <c r="F22" s="31">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.16666666666669999</v>
       </c>
       <c r="G22" s="31">
-        <f t="shared" si="3"/>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="2"/>
+        <v>0.16666666666669999</v>
       </c>
       <c r="H22" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="I22" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
     </row>
@@ -3812,38 +4153,38 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C26" s="31">
-        <f>SUM(C15:C22)</f>
-        <v>2.0999999999999996</v>
+        <f t="shared" ref="C26:I26" si="3">SUM(C15:C22)</f>
+        <v>2.1</v>
       </c>
       <c r="D26" s="31">
-        <f t="shared" ref="D26:I26" si="4">SUM(D15:D22)</f>
+        <f t="shared" si="3"/>
         <v>3.4750000000000001</v>
       </c>
       <c r="E26" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.7250000000000001</v>
       </c>
       <c r="F26" s="31">
-        <f t="shared" si="4"/>
-        <v>4.7333333333333334</v>
+        <f t="shared" si="3"/>
+        <v>4.7333333333332996</v>
       </c>
       <c r="G26" s="31">
-        <f t="shared" si="4"/>
-        <v>4.666666666666667</v>
+        <f t="shared" si="3"/>
+        <v>4.6666666666666998</v>
       </c>
       <c r="H26" s="31">
-        <f t="shared" si="4"/>
-        <v>3.3200000000000003</v>
+        <f t="shared" si="3"/>
+        <v>3.32</v>
       </c>
       <c r="I26" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.38750000000000001</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C27">
         <f>Member!$E11*'Characteristik analyse'!C26</f>
-        <v>2.0999999999999996</v>
+        <v>2.1</v>
       </c>
       <c r="D27" s="6">
         <f>Member!$E12*'Characteristik analyse'!D26</f>
@@ -3876,9 +4217,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:I13">
     <cfRule type="colorScale" priority="91">
@@ -3933,11 +4274,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -4039,7 +4380,7 @@
       </c>
       <c r="E6" s="8">
         <f>C6/3</f>
-        <v>2.9833333333333329</v>
+        <v>2.9833333333333001</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -4143,7 +4484,7 @@
       </c>
       <c r="E10" s="8">
         <f>C10/20</f>
-        <v>1.7600000000000002</v>
+        <v>1.76</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -4195,7 +4536,7 @@
       </c>
       <c r="E12" s="8">
         <f>C12/10</f>
-        <v>1.9989999999999999</v>
+        <v>1.9990000000000001</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
@@ -4247,7 +4588,7 @@
       </c>
       <c r="E14" s="8">
         <f>C14/3</f>
-        <v>6.6633333333333331</v>
+        <v>6.6633333333333002</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
@@ -4299,7 +4640,7 @@
       </c>
       <c r="E16" s="8">
         <f>C16/20</f>
-        <v>0.99949999999999994</v>
+        <v>0.99950000000000006</v>
       </c>
       <c r="F16" s="6">
         <v>0</v>
@@ -4336,7 +4677,7 @@
       </c>
       <c r="H17" s="32">
         <f>Tabelle4[[#This Row],[€ genutzt/Packung]]/Tabelle4[[#This Row],[€/Packung]]</f>
-        <v>9.9999999999999992E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -4345,14 +4686,14 @@
       </c>
       <c r="C18" s="9">
         <f>SUM(C4:C17)</f>
-        <v>217.15000000000003</v>
+        <v>217.15</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G18" s="9">
         <f>SUM(G4:G17)</f>
-        <v>22.084999999999997</v>
+        <v>22.085000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some warband info summary
</commit_message>
<xml_diff>
--- a/kai/kai-warband_orks_mostlyepic_goblins.xlsx
+++ b/kai/kai-warband_orks_mostlyepic_goblins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\Dropbox\Privat\Mordheim\kai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FEE43450-1D9E-4CD0-A325-69453EE09E8B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2EFEC395-0261-4913-9929-41E8AA67F63D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,9 +477,6 @@
     <t>Leader/Boss</t>
   </si>
   <si>
-    <t>Grumlock 'n Gazbag</t>
-  </si>
-  <si>
     <t>Far-Sight</t>
   </si>
   <si>
@@ -546,6 +543,9 @@
   </si>
   <si>
     <t>Ug'lash</t>
+  </si>
+  <si>
+    <t>Grumlok and Gazbag</t>
   </si>
 </sst>
 </file>
@@ -791,15 +791,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -839,66 +830,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -1010,6 +955,61 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1024,36 +1024,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="C21:U39" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ausrüstung gesamt"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Typ"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Range"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="S" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="S" dataDxfId="19"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SP"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="gold/stück"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Boss" dataDxfId="25">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Boss" dataDxfId="18">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="schamane" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="big'uns" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="goblin" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="squig" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="boy" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="troll" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="kosten" dataDxfId="18">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="schamane" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="big'uns" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="goblin" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="squig" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="boy" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="troll" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="kosten" dataDxfId="11">
       <calculatedColumnFormula>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="wunsch" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="wunsch" dataDxfId="10">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="zusatzkosten" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="zusatzkosten" dataDxfId="9">
       <calculatedColumnFormula>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gruppe" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Bewertung" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Warband Equip Rating" dataDxfId="13">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gruppe" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Bewertung" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Warband Equip Rating" dataDxfId="6">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1062,17 +1062,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle4" displayName="Tabelle4" ref="B3:G17" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle4" displayName="Tabelle4" ref="B3:G17" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B3:G17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Mögliche einheiten" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="€/Packung" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="€/Figur" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Mögliche einheiten" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="€/Packung" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="€/Figur" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Genutzte figuren"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="€ genutzt/Packung" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="€ genutzt/Packung" dataDxfId="1">
       <calculatedColumnFormula>E4*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Prozentuale Nutzung" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Prozentuale Nutzung" dataDxfId="0">
       <calculatedColumnFormula>Tabelle4[[#This Row],[€ genutzt/Packung]]/Tabelle4[[#This Row],[€/Packung]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1345,34 +1345,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="42" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="45"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.35">
       <c r="B2" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>149</v>
+      <c r="C2" s="56" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="42">
         <v>80</v>
       </c>
       <c r="E3" s="18"/>
@@ -1381,20 +1381,20 @@
       <c r="B4" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>135</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="46">
+        <v>160</v>
+      </c>
+      <c r="C5" s="43">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E5" s="18"/>
     </row>
@@ -1402,8 +1402,8 @@
       <c r="B6" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="45" t="s">
-        <v>151</v>
+      <c r="C6" s="42" t="s">
+        <v>150</v>
       </c>
       <c r="E6" s="18"/>
     </row>
@@ -1411,7 +1411,7 @@
       <c r="B7" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>145</v>
       </c>
       <c r="E7" s="18"/>
@@ -1420,7 +1420,7 @@
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="42">
         <f>'cost calculation'!H26</f>
         <v>15</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="42">
         <v>5</v>
       </c>
       <c r="D9" s="6"/>
@@ -1442,9 +1442,9 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
       <c r="B10" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="47">
+        <v>159</v>
+      </c>
+      <c r="C10" s="44">
         <v>20</v>
       </c>
       <c r="D10" s="6"/>
@@ -1452,10 +1452,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="39"/>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="56">
+      <c r="C11" s="53">
         <v>10</v>
       </c>
       <c r="D11" s="6"/>
@@ -1463,9 +1463,9 @@
     </row>
     <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="39"/>
-      <c r="C12" s="47">
-        <f>SUM(C2:C11)</f>
-        <v>135</v>
+      <c r="C12" s="44">
+        <f>C3+C8+C9+C10+C11</f>
+        <v>130</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>138</v>
@@ -1477,17 +1477,17 @@
     <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="39"/>
       <c r="B14"/>
-      <c r="C14" s="45"/>
+      <c r="C14" s="42"/>
       <c r="D14"/>
       <c r="E14"/>
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A15" s="39"/>
       <c r="B15" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="59" t="s">
-        <v>166</v>
+        <v>167</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1495,7 +1495,7 @@
       <c r="B16" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="45">
         <v>40</v>
       </c>
       <c r="E16" s="41"/>
@@ -1505,7 +1505,7 @@
       <c r="B17" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="42" t="s">
         <v>136</v>
       </c>
       <c r="E17" s="41"/>
@@ -1513,9 +1513,9 @@
     <row r="18" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="39"/>
       <c r="B18" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C18" s="49">
+        <v>160</v>
+      </c>
+      <c r="C18" s="46">
         <v>0</v>
       </c>
       <c r="E18" s="41"/>
@@ -1525,8 +1525,8 @@
       <c r="B19" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="52" t="s">
-        <v>152</v>
+      <c r="C19" s="49" t="s">
+        <v>151</v>
       </c>
       <c r="E19" s="41"/>
     </row>
@@ -1535,7 +1535,7 @@
       <c r="B20" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="42" t="s">
         <v>145</v>
       </c>
       <c r="E20" s="41"/>
@@ -1545,7 +1545,7 @@
       <c r="B21" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="45">
         <v>15</v>
       </c>
     </row>
@@ -1554,7 +1554,7 @@
       <c r="B22" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="45">
         <v>5</v>
       </c>
       <c r="D22" s="6"/>
@@ -1562,18 +1562,18 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="39"/>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23" s="51">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="39"/>
       <c r="B24" s="39"/>
-      <c r="C24" s="50">
-        <f>SUM(C16:C23)</f>
+      <c r="C24" s="47">
+        <f>C16+C21+C22+C23</f>
         <v>80</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -1584,24 +1584,24 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
-      <c r="C25" s="48"/>
+      <c r="C25" s="45"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="39"/>
       <c r="B26" s="39"/>
-      <c r="C26" s="48"/>
+      <c r="C26" s="45"/>
       <c r="D26"/>
       <c r="E26"/>
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A27" s="39"/>
       <c r="B27" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C27" s="59" t="s">
         <v>167</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1609,7 +1609,7 @@
       <c r="B28" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="51">
+      <c r="C28" s="48">
         <v>40</v>
       </c>
       <c r="E28" s="18"/>
@@ -1619,7 +1619,7 @@
       <c r="B29" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="42" t="s">
         <v>136</v>
       </c>
       <c r="E29" s="18"/>
@@ -1627,9 +1627,9 @@
     <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="39"/>
       <c r="B30" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C30" s="46">
+        <v>160</v>
+      </c>
+      <c r="C30" s="43">
         <v>0</v>
       </c>
       <c r="E30" s="18"/>
@@ -1639,8 +1639,8 @@
       <c r="B31" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="52" t="s">
-        <v>152</v>
+      <c r="C31" s="49" t="s">
+        <v>151</v>
       </c>
       <c r="E31" s="18"/>
     </row>
@@ -1649,7 +1649,7 @@
       <c r="B32" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="42" t="s">
         <v>145</v>
       </c>
       <c r="E32" s="18"/>
@@ -1658,7 +1658,7 @@
       <c r="B33" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="48">
+      <c r="C33" s="45">
         <v>5</v>
       </c>
     </row>
@@ -1666,22 +1666,22 @@
       <c r="B34" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="48">
+      <c r="C34" s="45">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="54">
+      <c r="C35" s="51">
         <v>20</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="39"/>
-      <c r="C36" s="50">
-        <f>SUM(C28:C35)</f>
+      <c r="C36" s="47">
+        <f>C28+C33+C34+C35</f>
         <v>75</v>
       </c>
       <c r="D36" s="6" t="s">
@@ -1691,29 +1691,29 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="39"/>
-      <c r="C37" s="48"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38"/>
-      <c r="C38" s="45"/>
+      <c r="C38" s="42"/>
       <c r="D38"/>
       <c r="E38"/>
     </row>
     <row r="39" spans="2:5" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="B39" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="59" t="s">
-        <v>171</v>
+        <v>167</v>
+      </c>
+      <c r="C39" s="56" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C40" s="45">
+      <c r="C40" s="42">
         <v>40</v>
       </c>
       <c r="E40" s="18"/>
@@ -1722,16 +1722,16 @@
       <c r="B41" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="42" t="s">
         <v>136</v>
       </c>
       <c r="E41" s="18"/>
     </row>
     <row r="42" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C42" s="46">
+        <v>160</v>
+      </c>
+      <c r="C42" s="43">
         <v>0</v>
       </c>
       <c r="E42" s="18"/>
@@ -1740,8 +1740,8 @@
       <c r="B43" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C43" s="52" t="s">
-        <v>152</v>
+      <c r="C43" s="49" t="s">
+        <v>151</v>
       </c>
       <c r="E43" s="18"/>
     </row>
@@ -1749,7 +1749,7 @@
       <c r="B44" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="42" t="s">
         <v>145</v>
       </c>
       <c r="E44" s="18"/>
@@ -1758,7 +1758,7 @@
       <c r="B45" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="45">
+      <c r="C45" s="42">
         <f>'cost calculation'!H23</f>
         <v>5</v>
       </c>
@@ -1767,24 +1767,24 @@
       <c r="B46" t="s">
         <v>134</v>
       </c>
-      <c r="C46" s="45">
+      <c r="C46" s="42">
         <f>'cost calculation'!H25</f>
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="56">
+      <c r="C47" s="53">
         <f>'cost calculation'!H37</f>
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
-      <c r="C48" s="47">
-        <f>SUM(C40:C47)</f>
+      <c r="C48" s="44">
+        <f>C40+C45+C47+C46</f>
         <v>75</v>
       </c>
       <c r="D48" s="6" t="s">
@@ -1793,27 +1793,27 @@
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="45"/>
+      <c r="C49" s="42"/>
     </row>
     <row r="50" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B50"/>
-      <c r="C50" s="45"/>
+      <c r="C50" s="42"/>
       <c r="D50"/>
       <c r="E50"/>
     </row>
     <row r="51" spans="1:5" ht="17.25" x14ac:dyDescent="0.35">
       <c r="B51" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C51" s="59" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="C51" s="56" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C52" s="45">
+      <c r="C52" s="42">
         <v>40</v>
       </c>
     </row>
@@ -1821,15 +1821,15 @@
       <c r="B53" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C53" s="45" t="s">
+      <c r="C53" s="42" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C54" s="45">
+        <v>160</v>
+      </c>
+      <c r="C54" s="42">
         <v>0</v>
       </c>
     </row>
@@ -1837,20 +1837,20 @@
       <c r="B55" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="45" t="s">
-        <v>154</v>
+      <c r="C55" s="42" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="55" t="s">
+      <c r="B56" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="C56" s="56" t="s">
-        <v>150</v>
+      <c r="C56" s="53" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C57" s="47">
+      <c r="C57" s="44">
         <f>C52</f>
         <v>40</v>
       </c>
@@ -1865,20 +1865,20 @@
     </row>
     <row r="60" spans="1:5" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B60" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C60" s="59" t="s">
-        <v>165</v>
+      <c r="C60" s="56" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C61" s="45">
+      <c r="C61" s="42">
         <v>15</v>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
       <c r="B62" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C62" s="45">
+      <c r="C62" s="42">
         <v>0</v>
       </c>
     </row>
@@ -1894,37 +1894,37 @@
       <c r="B63" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C63" s="45" t="s">
+      <c r="C63" s="42" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B64" s="58" t="s">
+      <c r="B64" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="C64" s="57" t="s">
-        <v>162</v>
+      <c r="C64" s="54" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="C65" s="45">
+      <c r="C66" s="53">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="C66" s="56">
-        <v>5</v>
-      </c>
-    </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C67" s="47">
-        <f>SUM(C61:C66)</f>
+      <c r="C67" s="44">
+        <f>C61+C65+C66</f>
         <v>25</v>
       </c>
       <c r="D67" t="s">
@@ -1935,15 +1935,15 @@
       <c r="B69" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="59" t="s">
-        <v>163</v>
+      <c r="C69" s="56" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="45">
+      <c r="C70" s="42">
         <v>15</v>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
       <c r="B71" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C71" s="45">
+      <c r="C71" s="42">
         <v>0</v>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       <c r="B72" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C72" s="45" t="s">
+      <c r="C72" s="42" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1967,29 +1967,29 @@
       <c r="B73" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C73" s="45" t="s">
-        <v>159</v>
+      <c r="C73" s="42" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C74" s="45">
+        <v>154</v>
+      </c>
+      <c r="C74" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="55" t="s">
-        <v>158</v>
-      </c>
-      <c r="C75" s="56">
+      <c r="B75" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="53">
         <v>10</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C76" s="47">
-        <f>C75+C70+C74</f>
+      <c r="C76" s="44">
+        <f>C70+C74+C75</f>
         <v>25</v>
       </c>
       <c r="D76" t="s">
@@ -2006,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD120"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2158,7 +2158,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="57" t="s">
         <v>81</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -2185,7 +2185,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="42"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="6" t="s">
         <v>83</v>
       </c>
@@ -2210,7 +2210,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="42"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="6" t="s">
         <v>84</v>
       </c>
@@ -2229,7 +2229,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="57" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -2250,7 +2250,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="42"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="6" t="s">
         <v>86</v>
       </c>
@@ -2269,7 +2269,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="42"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="6" t="s">
         <v>87</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="42"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
@@ -2323,30 +2323,30 @@
     <row r="19" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17"/>
       <c r="F19" s="1"/>
-      <c r="I19" s="43" t="s">
+      <c r="I19" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
     </row>
     <row r="20" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43" t="s">
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
       <c r="T20" s="6" t="s">
         <v>122</v>
       </c>
@@ -3711,7 +3711,7 @@
     <mergeCell ref="L20:O20"/>
   </mergeCells>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="6" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="55" operator="greaterThan">
       <formula>$C$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3812,32 +3812,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:O22">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I39">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:O39">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:O39">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E17">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3890,17 +3890,17 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44" t="s">
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="13"/>
@@ -3932,10 +3932,10 @@
         <f>'cost calculation'!C17</f>
         <v>troll</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="58"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">

</xml_diff>

<commit_message>
Fernkampf für die Orks.
</commit_message>
<xml_diff>
--- a/kai/kai-warband_orks_mostlyepic_goblins.xlsx
+++ b/kai/kai-warband_orks_mostlyepic_goblins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klaute\Dropbox\Privat\Mordheim\kai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\Dropbox\Privat\Mordheim\kai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{765DA45B-7F27-4522-A684-EF91B279DF32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8264E49-FE5F-4208-B730-A0ABAD63F825}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="warband detail" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Characteristik analyse" sheetId="2" r:id="rId3"/>
     <sheet name="Boxen" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>gold</t>
   </si>
@@ -475,6 +475,9 @@
   </si>
   <si>
     <t>Leader/Boss</t>
+  </si>
+  <si>
+    <t>Grumlock 'n Gazbag</t>
   </si>
   <si>
     <t>Far-Sight</t>
@@ -543,9 +546,6 @@
   </si>
   <si>
     <t>Ug'lash</t>
-  </si>
-  <si>
-    <t>Grumlok and Gazbag</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1357,18 +1357,18 @@
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="1" s="6">
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="2" ht="17">
       <c r="B2" s="23" t="s">
         <v>148</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" s="6">
       <c r="B3" s="6" t="s">
         <v>146</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" customFormat="1" s="6">
       <c r="B4" s="6" t="s">
         <v>147</v>
       </c>
@@ -1386,28 +1386,28 @@
       </c>
       <c r="E4" s="18"/>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" customFormat="1" s="6">
       <c r="B5" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C5" s="43">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" customFormat="1" s="6">
       <c r="B6" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" customFormat="1" s="6">
       <c r="B7" s="6" t="s">
         <v>143</v>
       </c>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="39"/>
       <c r="B9" s="6" t="s">
         <v>8</v>
@@ -1439,10 +1439,10 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="39"/>
       <c r="B10" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C10" s="44">
         <v>20</v>
@@ -1450,7 +1450,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="39"/>
       <c r="B11" s="52" t="s">
         <v>7</v>
@@ -1461,36 +1461,33 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" customFormat="1" s="6">
       <c r="A12" s="39"/>
       <c r="C12" s="44">
-        <f>C3+C8+C9+C10+C11</f>
-        <v>130</v>
+        <f>SUM(C2:C11)</f>
+        <v>135</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="39"/>
     </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" customFormat="1" s="6">
       <c r="A14" s="39"/>
-      <c r="B14"/>
       <c r="C14" s="42"/>
-      <c r="D14"/>
-      <c r="E14"/>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" ht="17" customFormat="1" s="6">
       <c r="A15" s="39"/>
       <c r="B15" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" s="6">
       <c r="A16" s="39"/>
       <c r="B16" s="6" t="s">
         <v>146</v>
@@ -1500,7 +1497,7 @@
       </c>
       <c r="E16" s="41"/>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="1" s="6">
       <c r="A17" s="39"/>
       <c r="B17" s="6" t="s">
         <v>147</v>
@@ -1510,27 +1507,27 @@
       </c>
       <c r="E17" s="41"/>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="1" s="6">
       <c r="A18" s="39"/>
       <c r="B18" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C18" s="46">
         <v>0</v>
       </c>
       <c r="E18" s="41"/>
     </row>
-    <row r="19" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="1" s="6">
       <c r="A19" s="39"/>
       <c r="B19" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E19" s="41"/>
     </row>
-    <row r="20" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" customFormat="1" s="6">
       <c r="A20" s="39"/>
       <c r="B20" s="6" t="s">
         <v>143</v>
@@ -1540,7 +1537,7 @@
       </c>
       <c r="E20" s="41"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="39"/>
       <c r="B21" s="40" t="s">
         <v>3</v>
@@ -1549,7 +1546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="39"/>
       <c r="B22" s="40" t="s">
         <v>8</v>
@@ -1560,7 +1557,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="39"/>
       <c r="B23" s="50" t="s">
         <v>6</v>
@@ -1569,11 +1566,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="39"/>
       <c r="B24" s="39"/>
       <c r="C24" s="47">
-        <f>C16+C21+C22+C23</f>
+        <f>SUM(C16:C23)</f>
         <v>80</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -1581,30 +1578,28 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
       <c r="C25" s="45"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" customFormat="1" s="6">
       <c r="A26" s="39"/>
       <c r="B26" s="39"/>
       <c r="C26" s="45"/>
-      <c r="D26"/>
-      <c r="E26"/>
-    </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" ht="17" customFormat="1" s="6">
       <c r="A27" s="39"/>
       <c r="B27" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="56" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" customFormat="1" s="6">
       <c r="A28" s="39"/>
       <c r="B28" s="6" t="s">
         <v>146</v>
@@ -1614,7 +1609,7 @@
       </c>
       <c r="E28" s="18"/>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" customFormat="1" s="6">
       <c r="A29" s="39"/>
       <c r="B29" s="6" t="s">
         <v>147</v>
@@ -1624,27 +1619,27 @@
       </c>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" customFormat="1" s="6">
       <c r="A30" s="39"/>
       <c r="B30" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C30" s="43">
         <v>0</v>
       </c>
       <c r="E30" s="18"/>
     </row>
-    <row r="31" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" customFormat="1" s="6">
       <c r="A31" s="39"/>
       <c r="B31" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E31" s="18"/>
     </row>
-    <row r="32" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" customFormat="1" s="6">
       <c r="A32" s="39"/>
       <c r="B32" s="6" t="s">
         <v>143</v>
@@ -1654,7 +1649,7 @@
       </c>
       <c r="E32" s="18"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="B33" s="39" t="s">
         <v>1</v>
       </c>
@@ -1662,7 +1657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="B34" s="39" t="s">
         <v>2</v>
       </c>
@@ -1670,7 +1665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="B35" s="50" t="s">
         <v>6</v>
       </c>
@@ -1678,10 +1673,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="B36" s="39"/>
       <c r="C36" s="47">
-        <f>C28+C33+C34+C35</f>
+        <f>SUM(C28:C35)</f>
         <v>75</v>
       </c>
       <c r="D36" s="6" t="s">
@@ -1689,27 +1684,24 @@
       </c>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="B37" s="39"/>
       <c r="C37" s="45"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B38"/>
+    <row r="38" customFormat="1" s="6">
       <c r="C38" s="42"/>
-      <c r="D38"/>
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="2:5" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" ht="17" customFormat="1" s="6">
       <c r="B39" s="23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" customFormat="1" s="6">
       <c r="B40" s="6" t="s">
         <v>146</v>
       </c>
@@ -1718,7 +1710,7 @@
       </c>
       <c r="E40" s="18"/>
     </row>
-    <row r="41" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" customFormat="1" s="6">
       <c r="B41" s="6" t="s">
         <v>147</v>
       </c>
@@ -1727,25 +1719,25 @@
       </c>
       <c r="E41" s="18"/>
     </row>
-    <row r="42" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" customFormat="1" s="6">
       <c r="B42" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C42" s="43">
         <v>0</v>
       </c>
       <c r="E42" s="18"/>
     </row>
-    <row r="43" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" customFormat="1" s="6">
       <c r="B43" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C43" s="49" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E43" s="18"/>
     </row>
-    <row r="44" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" customFormat="1" s="6">
       <c r="B44" s="6" t="s">
         <v>143</v>
       </c>
@@ -1754,7 +1746,7 @@
       </c>
       <c r="E44" s="18"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="B45" t="s">
         <v>1</v>
       </c>
@@ -1763,7 +1755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="B46" t="s">
         <v>134</v>
       </c>
@@ -1772,7 +1764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="B47" s="52" t="s">
         <v>6</v>
       </c>
@@ -1781,10 +1773,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="B48" s="6"/>
       <c r="C48" s="44">
-        <f>C40+C45+C47+C46</f>
+        <f>SUM(C40:C47)</f>
         <v>75</v>
       </c>
       <c r="D48" s="6" t="s">
@@ -1792,24 +1784,21 @@
       </c>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" customFormat="1" s="6">
       <c r="C49" s="42"/>
     </row>
-    <row r="50" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B50"/>
+    <row r="50" customFormat="1" s="6">
       <c r="C50" s="42"/>
-      <c r="D50"/>
-      <c r="E50"/>
-    </row>
-    <row r="51" spans="1:5" ht="17.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" ht="17">
       <c r="B51" s="23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C51" s="56" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" customFormat="1" s="6">
       <c r="B52" s="6" t="s">
         <v>146</v>
       </c>
@@ -1817,7 +1806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" customFormat="1" s="6">
       <c r="B53" s="6" t="s">
         <v>147</v>
       </c>
@@ -1825,31 +1814,31 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" customFormat="1" s="6">
       <c r="B54" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C54" s="42">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" customFormat="1" s="6">
       <c r="B55" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" customFormat="1" s="6">
       <c r="B56" s="52" t="s">
         <v>143</v>
       </c>
       <c r="C56" s="53" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57">
       <c r="C57" s="44">
         <f>C52</f>
         <v>40</v>
@@ -1858,23 +1847,23 @@
         <v>138</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="B58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="60" ht="17">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B60" s="23" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="56" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" customFormat="1" s="6">
       <c r="B61" s="6" t="s">
         <v>146</v>
       </c>
@@ -1882,7 +1871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" customFormat="1" s="6">
       <c r="B62" s="6" t="s">
         <v>147</v>
       </c>
@@ -1890,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" customFormat="1" s="6">
       <c r="B63" s="6" t="s">
         <v>144</v>
       </c>
@@ -1898,48 +1887,48 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="6" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="64" ht="38" customFormat="1" s="6">
       <c r="B64" s="55" t="s">
         <v>143</v>
       </c>
       <c r="C64" s="54" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65">
       <c r="B65" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C65" s="42">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="B66" s="52" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C66" s="53">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="C67" s="44">
-        <f>C61+C65+C66</f>
+        <f>SUM(C61:C66)</f>
         <v>25</v>
       </c>
       <c r="D67" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="2:4" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="69" ht="17">
       <c r="B69" s="23" t="s">
         <v>139</v>
       </c>
       <c r="C69" s="56" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" customFormat="1" s="6">
       <c r="B70" s="6" t="s">
         <v>146</v>
       </c>
@@ -1947,7 +1936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" customFormat="1" s="6">
       <c r="B71" s="6" t="s">
         <v>147</v>
       </c>
@@ -1955,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" customFormat="1" s="6">
       <c r="B72" s="6" t="s">
         <v>144</v>
       </c>
@@ -1963,33 +1952,33 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="B73" s="6" t="s">
         <v>143</v>
       </c>
       <c r="C73" s="42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" customFormat="1" s="6">
+      <c r="B74" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="1" s="6">
+      <c r="B75" s="52" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C74" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="52" t="s">
-        <v>157</v>
       </c>
       <c r="C75" s="53">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="C76" s="44">
-        <f>C70+C74+C75</f>
+        <f>C75+C70+C74</f>
         <v>25</v>
       </c>
       <c r="D76" t="s">
@@ -2006,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD120"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="J19" zoomScaleNormal="45" workbookViewId="0" tabSelected="true" zoomScale="45">
+      <selection activeCell="I39" sqref="I39" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2033,20 +2022,23 @@
     <col min="19" max="19" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="6.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="55.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="13" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" ht="18">
       <c r="B2" s="11" t="s">
         <v>16</v>
       </c>
@@ -2059,7 +2051,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="3" spans="2:18" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" ht="18" customFormat="1" s="6">
       <c r="B3" s="11" t="s">
         <v>129</v>
       </c>
@@ -2072,7 +2064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="H4" s="11" t="s">
         <v>60</v>
       </c>
@@ -2081,7 +2073,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="2:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" customFormat="1" s="6">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -2096,7 +2088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" customFormat="1" s="6">
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2109,18 +2101,18 @@
       </c>
       <c r="I6" s="38">
         <f>U40</f>
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J6" s="6">
         <f>U41</f>
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="K6" s="6">
         <f>U42</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" ht="15">
       <c r="B7" s="26" t="s">
         <v>15</v>
       </c>
@@ -2130,11 +2122,11 @@
       </c>
       <c r="I7" s="2">
         <f>I3+(I6+I4)*I5</f>
-        <v>769</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" s="6"/>
+    <row r="10">
       <c r="C10" s="12" t="s">
         <v>17</v>
       </c>
@@ -2157,7 +2149,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="B11" s="57" t="s">
         <v>81</v>
       </c>
@@ -2174,7 +2166,7 @@
         <v>20</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G17" si="0">E11*D11</f>
+        <f>E11*D11</f>
         <v>80</v>
       </c>
       <c r="Q11" s="6" t="s">
@@ -2184,7 +2176,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="57"/>
       <c r="C12" s="6" t="s">
         <v>83</v>
@@ -2199,7 +2191,7 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f>E12*D12</f>
         <v>40</v>
       </c>
       <c r="Q12" s="6" t="s">
@@ -2209,7 +2201,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="B13" s="57"/>
       <c r="C13" s="6" t="s">
         <v>84</v>
@@ -2224,11 +2216,11 @@
         <v>15</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f>E13*D13</f>
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="B14" s="57" t="s">
         <v>46</v>
       </c>
@@ -2245,11 +2237,11 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f>E14*D14</f>
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="B15" s="57"/>
       <c r="C15" s="6" t="s">
         <v>86</v>
@@ -2264,11 +2256,11 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+        <f>E15*D15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="B16" s="57"/>
       <c r="C16" s="6" t="s">
         <v>87</v>
@@ -2283,11 +2275,11 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+        <f>E16*D16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="B17" s="57"/>
       <c r="C17" s="5" t="s">
         <v>11</v>
@@ -2302,11 +2294,11 @@
         <v>0</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+        <f>E17*D17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" ht="15">
       <c r="C18" s="16" t="s">
         <v>43</v>
       </c>
@@ -2320,7 +2312,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="1" s="6">
       <c r="B19" s="17"/>
       <c r="F19" s="1"/>
       <c r="I19" s="58" t="s">
@@ -2333,7 +2325,7 @@
       <c r="N19" s="58"/>
       <c r="O19" s="58"/>
     </row>
-    <row r="20" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" ht="15">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="I20" s="58" t="s">
@@ -2351,7 +2343,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="1" s="6">
       <c r="C21" s="12" t="s">
         <v>76</v>
       </c>
@@ -2410,7 +2402,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" customFormat="1" s="6">
       <c r="C22" s="6" t="s">
         <v>9</v>
       </c>
@@ -2467,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" customFormat="1" s="6">
       <c r="C23" s="6" t="s">
         <v>1</v>
       </c>
@@ -2524,7 +2516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" customFormat="1" s="6">
       <c r="C24" s="6" t="s">
         <v>88</v>
       </c>
@@ -2583,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" customFormat="1" s="6">
       <c r="C25" s="6" t="s">
         <v>2</v>
       </c>
@@ -2642,7 +2634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" customFormat="1" s="6">
       <c r="C26" s="6" t="s">
         <v>3</v>
       </c>
@@ -2665,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="6">
         <v>0</v>
@@ -2681,7 +2673,7 @@
       </c>
       <c r="P26" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -2698,10 +2690,10 @@
       </c>
       <c r="U26" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="1" s="6">
       <c r="C27" s="6" t="s">
         <v>94</v>
       </c>
@@ -2724,7 +2716,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="6">
         <v>0</v>
@@ -2740,7 +2732,7 @@
       </c>
       <c r="P27" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q27" s="6">
         <v>0</v>
@@ -2757,10 +2749,10 @@
       </c>
       <c r="U27" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1" s="6">
       <c r="C28" s="6" t="s">
         <v>97</v>
       </c>
@@ -2814,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" customFormat="1" s="6">
       <c r="C29" s="6" t="s">
         <v>4</v>
       </c>
@@ -2876,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" customFormat="1" s="6">
       <c r="C30" s="6" t="s">
         <v>5</v>
       </c>
@@ -2935,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" customFormat="1" s="6">
       <c r="C31" s="6" t="s">
         <v>99</v>
       </c>
@@ -2989,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" customFormat="1" s="6">
       <c r="C32" s="6" t="s">
         <v>10</v>
       </c>
@@ -3048,7 +3040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" customFormat="1" s="6">
       <c r="C33" s="6" t="s">
         <v>100</v>
       </c>
@@ -3074,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M33" s="6">
         <v>0</v>
@@ -3087,7 +3079,7 @@
       </c>
       <c r="P33" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q33" s="6">
         <v>0</v>
@@ -3104,10 +3096,10 @@
       </c>
       <c r="U33" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" customFormat="1" s="6">
       <c r="C34" s="6" t="s">
         <v>102</v>
       </c>
@@ -3164,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" customFormat="1" s="6">
       <c r="C35" s="6" t="s">
         <v>104</v>
       </c>
@@ -3223,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" customFormat="1" s="6">
       <c r="C36" s="34" t="s">
         <v>106</v>
       </c>
@@ -3279,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" customFormat="1" s="6">
       <c r="C37" s="6" t="s">
         <v>6</v>
       </c>
@@ -3336,7 +3328,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" customFormat="1" s="6">
       <c r="C38" s="6" t="s">
         <v>8</v>
       </c>
@@ -3358,10 +3350,10 @@
         <v>0</v>
       </c>
       <c r="K38" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M38" s="6">
         <v>0</v>
@@ -3394,7 +3386,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" customFormat="1" s="6">
       <c r="C39" s="34" t="s">
         <v>7</v>
       </c>
@@ -3407,9 +3399,7 @@
       <c r="H39" s="34">
         <v>10</v>
       </c>
-      <c r="I39" s="6">
-        <v>1</v>
-      </c>
+      <c r="I39" s="6"/>
       <c r="J39" s="6">
         <v>0</v>
       </c>
@@ -3430,7 +3420,7 @@
       </c>
       <c r="P39" s="6">
         <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="6">
         <v>0</v>
@@ -3447,10 +3437,10 @@
       </c>
       <c r="U39" s="30">
         <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="3:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="15" customFormat="1" s="6">
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
       <c r="E40" s="34"/>
@@ -3458,31 +3448,31 @@
       <c r="G40" s="34"/>
       <c r="H40" s="34"/>
       <c r="I40" s="3">
-        <f t="shared" ref="I40:O40" si="1">I22*$H22+I23*$H23+I24*$H24+I25*$H25+I26*$H26+I27*$H27+I28*$H28+I29*$H29+I30*$H30+I31*$H31+I32*$H32+I33*$H33+I34*$H34+I35*$H35+I36*$H36+I37*$H37+I38*$H38+I39*$H39</f>
-        <v>50</v>
+        <f>I22*$H22+I23*$H23+I24*$H24+I25*$H25+I26*$H26+I27*$H27+I28*$H28+I29*$H29+I30*$H30+I31*$H31+I32*$H32+I33*$H33+I34*$H34+I35*$H35+I36*$H36+I37*$H37+I38*$H38+I39*$H39</f>
+        <v>40</v>
       </c>
       <c r="J40" s="3">
-        <f t="shared" si="1"/>
+        <f>J22*$H22+J23*$H23+J24*$H24+J25*$H25+J26*$H26+J27*$H27+J28*$H28+J29*$H29+J30*$H30+J31*$H31+J32*$H32+J33*$H33+J34*$H34+J35*$H35+J36*$H36+J37*$H37+J38*$H38+J39*$H39</f>
         <v>0</v>
       </c>
       <c r="K40" s="3">
-        <f t="shared" si="1"/>
-        <v>110</v>
+        <f>K22*$H22+K23*$H23+K24*$H24+K25*$H25+K26*$H26+K27*$H27+K28*$H28+K29*$H29+K30*$H30+K31*$H31+K32*$H32+K33*$H33+K34*$H34+K35*$H35+K36*$H36+K37*$H37+K38*$H38+K39*$H39</f>
+        <v>100</v>
       </c>
       <c r="L40" s="3">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f>L22*$H22+L23*$H23+L24*$H24+L25*$H25+L26*$H26+L27*$H27+L28*$H28+L29*$H29+L30*$H30+L31*$H31+L32*$H32+L33*$H33+L34*$H34+L35*$H35+L36*$H36+L37*$H37+L38*$H38+L39*$H39</f>
+        <v>60</v>
       </c>
       <c r="M40" s="3">
-        <f t="shared" si="1"/>
+        <f>M22*$H22+M23*$H23+M24*$H24+M25*$H25+M26*$H26+M27*$H27+M28*$H28+M29*$H29+M30*$H30+M31*$H31+M32*$H32+M33*$H33+M34*$H34+M35*$H35+M36*$H36+M37*$H37+M38*$H38+M39*$H39</f>
         <v>0</v>
       </c>
       <c r="N40" s="3">
-        <f t="shared" si="1"/>
+        <f>N22*$H22+N23*$H23+N24*$H24+N25*$H25+N26*$H26+N27*$H27+N28*$H28+N29*$H29+N30*$H30+N31*$H31+N32*$H32+N33*$H33+N34*$H34+N35*$H35+N36*$H36+N37*$H37+N38*$H38+N39*$H39</f>
         <v>0</v>
       </c>
       <c r="O40" s="3">
-        <f t="shared" si="1"/>
+        <f>O22*$H22+O23*$H23+O24*$H24+O25*$H25+O26*$H26+O27*$H27+O28*$H28+O29*$H29+O30*$H30+O31*$H31+O32*$H32+O33*$H33+O34*$H34+O35*$H35+O36*$H36+O37*$H37+O38*$H38+O39*$H39</f>
         <v>0</v>
       </c>
       <c r="P40" s="2">
@@ -3500,10 +3490,10 @@
       </c>
       <c r="U40" s="2">
         <f>SUM(Tabelle2[Warband Equip Rating])</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" customFormat="1" s="6">
       <c r="F41" s="29"/>
       <c r="S41" s="30"/>
       <c r="T41" s="6" t="s">
@@ -3511,10 +3501,10 @@
       </c>
       <c r="U41" s="6">
         <f>SUM(U22:U36)</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" customFormat="1" s="6">
       <c r="F42" s="29"/>
       <c r="S42" s="30"/>
       <c r="T42" s="6" t="s">
@@ -3522,10 +3512,10 @@
       </c>
       <c r="U42" s="6">
         <f>SUM(U37:U39)</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" customFormat="1" s="6">
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
@@ -3544,27 +3534,27 @@
       <c r="R43" s="34"/>
       <c r="S43" s="36"/>
     </row>
-    <row r="44" spans="3:21" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" ht="15" customFormat="1" s="6">
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" customFormat="1" s="6"/>
+    <row r="46" customFormat="1" s="6"/>
+    <row r="47" customFormat="1" s="6"/>
+    <row r="48" customFormat="1" s="6"/>
+    <row r="49" customFormat="1" s="6"/>
+    <row r="50" customFormat="1" s="6"/>
+    <row r="51" customFormat="1" s="6"/>
+    <row r="52" customFormat="1" s="6">
       <c r="V52" s="1"/>
     </row>
-    <row r="53" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" customFormat="1" s="6">
       <c r="V53" s="1"/>
     </row>
-    <row r="54" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="F54" s="6"/>
@@ -3573,57 +3563,57 @@
       <c r="I54" s="6"/>
       <c r="P54" s="6"/>
     </row>
-    <row r="55" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" customFormat="1" s="6"/>
+    <row r="56" customFormat="1" s="6"/>
+    <row r="57" customFormat="1" s="6"/>
+    <row r="58" customFormat="1" s="6">
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
     </row>
-    <row r="59" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="3:22" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="82" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="83" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="84" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="85" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="86" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="87" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="88" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="89" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="90" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="91" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="92" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="93" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="94" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="95" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="96" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="97" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="98" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="99" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="100" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="101" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="59" customFormat="1" s="6"/>
+    <row r="60" customFormat="1" s="6"/>
+    <row r="61" customFormat="1" s="6"/>
+    <row r="62" customFormat="1" s="6"/>
+    <row r="63" customFormat="1" s="6"/>
+    <row r="64" customFormat="1" s="6"/>
+    <row r="65" customFormat="1" s="6"/>
+    <row r="66" customFormat="1" s="6"/>
+    <row r="67" customFormat="1" s="6"/>
+    <row r="68" customFormat="1" s="6"/>
+    <row r="69" customFormat="1" s="6"/>
+    <row r="70" customFormat="1" s="6"/>
+    <row r="71" customFormat="1" s="6"/>
+    <row r="72" customFormat="1" s="6"/>
+    <row r="73" customFormat="1" s="6"/>
+    <row r="74" customFormat="1" s="6"/>
+    <row r="75" customFormat="1" s="6"/>
+    <row r="76" customFormat="1" s="6"/>
+    <row r="77" customFormat="1" s="6"/>
+    <row r="78" customFormat="1" s="6"/>
+    <row r="79" customFormat="1" s="6"/>
+    <row r="80" customFormat="1" s="6"/>
+    <row r="81" customFormat="1" s="6"/>
+    <row r="82" customFormat="1" s="6"/>
+    <row r="83" customFormat="1" s="6"/>
+    <row r="84" customFormat="1" s="6"/>
+    <row r="85" customFormat="1" s="6"/>
+    <row r="86" customFormat="1" s="6"/>
+    <row r="87" customFormat="1" s="6"/>
+    <row r="88" customFormat="1" s="6"/>
+    <row r="89" customFormat="1" s="6"/>
+    <row r="90" customFormat="1" s="6"/>
+    <row r="91" customFormat="1" s="6"/>
+    <row r="92" customFormat="1" s="6"/>
+    <row r="93" customFormat="1" s="6"/>
+    <row r="94" customFormat="1" s="6"/>
+    <row r="95" customFormat="1" s="6"/>
+    <row r="96" customFormat="1" s="6"/>
+    <row r="97" customFormat="1" s="6"/>
+    <row r="98" customFormat="1" s="6"/>
+    <row r="99" customFormat="1" s="6"/>
+    <row r="100" customFormat="1" s="6"/>
+    <row r="101">
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
       <c r="F101" s="6"/>
@@ -3632,7 +3622,7 @@
       <c r="I101" s="6"/>
       <c r="P101" s="6"/>
     </row>
-    <row r="102" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="102">
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
       <c r="F102" s="6"/>
@@ -3641,7 +3631,7 @@
       <c r="I102" s="6"/>
       <c r="P102" s="6"/>
     </row>
-    <row r="103" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="103">
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
       <c r="F103" s="6"/>
@@ -3650,7 +3640,7 @@
       <c r="I103" s="6"/>
       <c r="P103" s="6"/>
     </row>
-    <row r="104" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="104">
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="F104" s="6"/>
@@ -3659,14 +3649,14 @@
       <c r="I104" s="6"/>
       <c r="P104" s="6"/>
     </row>
-    <row r="110" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="111" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="112" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="113" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="114" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="115" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="116" spans="3:16" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="117" spans="3:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" customFormat="1" s="6"/>
+    <row r="111" customFormat="1" s="6"/>
+    <row r="112" customFormat="1" s="6"/>
+    <row r="113" customFormat="1" s="6"/>
+    <row r="114" customFormat="1" s="6"/>
+    <row r="115" customFormat="1" s="6"/>
+    <row r="116" customFormat="1" s="6"/>
+    <row r="117" customHeight="1" ht="12">
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
       <c r="F117" s="6"/>
@@ -3675,7 +3665,7 @@
       <c r="I117" s="6"/>
       <c r="P117" s="6"/>
     </row>
-    <row r="118" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="118">
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="F118" s="6"/>
@@ -3684,7 +3674,7 @@
       <c r="I118" s="6"/>
       <c r="P118" s="6"/>
     </row>
-    <row r="119" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="119">
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="F119" s="6"/>
@@ -3693,7 +3683,7 @@
       <c r="I119" s="6"/>
       <c r="P119" s="6"/>
     </row>
-    <row r="120" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="120">
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="F120" s="6"/>
@@ -3884,12 +3874,12 @@
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" ht="15">
       <c r="B2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" ht="15">
       <c r="C3" s="59" t="s">
         <v>45</v>
       </c>
@@ -3902,7 +3892,7 @@
       <c r="H3" s="59"/>
       <c r="I3" s="59"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="B4" s="13"/>
       <c r="C4" s="12" t="str">
         <f>'cost calculation'!C11</f>
@@ -3937,7 +3927,7 @@
       </c>
       <c r="L4" s="58"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="B5" s="14" t="s">
         <v>22</v>
       </c>
@@ -3969,7 +3959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="14" t="s">
         <v>23</v>
       </c>
@@ -3998,11 +3988,11 @@
         <v>10</v>
       </c>
       <c r="L6" s="25">
-        <f t="shared" ref="L6:L11" si="0">K6-3</f>
+        <f>K6-3</f>
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="14" t="s">
         <v>24</v>
       </c>
@@ -4031,11 +4021,11 @@
         <v>10</v>
       </c>
       <c r="L7" s="25">
-        <f t="shared" si="0"/>
+        <f>K7-3</f>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="14" t="s">
         <v>25</v>
       </c>
@@ -4064,11 +4054,11 @@
         <v>8</v>
       </c>
       <c r="L8" s="25">
-        <f t="shared" si="0"/>
+        <f>K8-3</f>
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="B9" s="14" t="s">
         <v>26</v>
       </c>
@@ -4097,11 +4087,11 @@
         <v>8</v>
       </c>
       <c r="L9" s="25">
-        <f t="shared" si="0"/>
+        <f>K9-3</f>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="B10" s="14" t="s">
         <v>27</v>
       </c>
@@ -4130,11 +4120,11 @@
         <v>3</v>
       </c>
       <c r="L10" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+        <f>K10-3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="B11" s="14" t="s">
         <v>28</v>
       </c>
@@ -4163,11 +4153,11 @@
         <v>4</v>
       </c>
       <c r="L11" s="25">
-        <f t="shared" si="0"/>
+        <f>K11-3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="14" t="s">
         <v>29</v>
       </c>
@@ -4199,7 +4189,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="B13" s="14" t="s">
         <v>30</v>
       </c>
@@ -4231,7 +4221,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -4241,271 +4231,271 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="B15" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="31">
-        <f t="shared" ref="C15:E22" si="1">$K6*C6/C$24</f>
+        <f>$K6*C6/C$24</f>
         <v>0.5</v>
       </c>
       <c r="D15" s="31">
-        <f t="shared" si="1"/>
+        <f>$K6*D6/D$24</f>
         <v>0.75</v>
       </c>
       <c r="E15" s="31">
-        <f t="shared" si="1"/>
+        <f>$K6*E6/E$24</f>
         <v>1</v>
       </c>
       <c r="F15" s="31">
-        <f t="shared" ref="F15:I22" si="2">$L6*F6/F$24</f>
-        <v>0.93333333333330004</v>
+        <f>$L6*F6/F$24</f>
+        <v>0.9333333333333</v>
       </c>
       <c r="G15" s="31">
-        <f t="shared" si="2"/>
+        <f>$L6*G6/G$24</f>
         <v>1.8666666666667</v>
       </c>
       <c r="H15" s="31">
-        <f t="shared" si="2"/>
+        <f>$L6*H6/H$24</f>
         <v>0.84</v>
       </c>
       <c r="I15" s="31">
-        <f t="shared" si="2"/>
+        <f>$L6*I6/I$24</f>
         <v>0.105</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="B16" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="31">
-        <f t="shared" si="1"/>
+        <f>$K7*C7/C$24</f>
         <v>0.5</v>
       </c>
       <c r="D16" s="31">
-        <f t="shared" si="1"/>
+        <f>$K7*D7/D$24</f>
         <v>0.75</v>
       </c>
       <c r="E16" s="31">
-        <f t="shared" si="1"/>
+        <f>$K7*E7/E$24</f>
         <v>0.75</v>
       </c>
       <c r="F16" s="31">
-        <f t="shared" si="2"/>
+        <f>$L7*F7/F$24</f>
         <v>1.4</v>
       </c>
       <c r="G16" s="31">
-        <f t="shared" si="2"/>
+        <f>$L7*G7/G$24</f>
         <v>0</v>
       </c>
       <c r="H16" s="31">
-        <f t="shared" si="2"/>
+        <f>$L7*H7/H$24</f>
         <v>0.84</v>
       </c>
       <c r="I16" s="31">
-        <f t="shared" si="2"/>
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+        <f>$L7*I7/I$24</f>
+        <v>0.035</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="B17" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="31">
-        <f t="shared" si="1"/>
+        <f>$K8*C8/C$24</f>
         <v>0.4</v>
       </c>
       <c r="D17" s="31">
-        <f t="shared" si="1"/>
+        <f>$K8*D8/D$24</f>
         <v>0.6</v>
       </c>
       <c r="E17" s="31">
-        <f t="shared" si="1"/>
+        <f>$K8*E8/E$24</f>
         <v>0.6</v>
       </c>
       <c r="F17" s="31">
-        <f t="shared" si="2"/>
+        <f>$L8*F8/F$24</f>
         <v>1</v>
       </c>
       <c r="G17" s="31">
-        <f t="shared" si="2"/>
+        <f>$L8*G8/G$24</f>
         <v>1.3333333333333</v>
       </c>
       <c r="H17" s="31">
-        <f t="shared" si="2"/>
+        <f>$L8*H8/H$24</f>
         <v>0.6</v>
       </c>
       <c r="I17" s="31">
-        <f t="shared" si="2"/>
+        <f>$L8*I8/I$24</f>
         <v>0.125</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="B18" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="31">
-        <f t="shared" si="1"/>
+        <f>$K9*C9/C$24</f>
         <v>0.4</v>
       </c>
       <c r="D18" s="31">
-        <f t="shared" si="1"/>
+        <f>$K9*D9/D$24</f>
         <v>0.8</v>
       </c>
       <c r="E18" s="31">
-        <f t="shared" si="1"/>
+        <f>$K9*E9/E$24</f>
         <v>0.8</v>
       </c>
       <c r="F18" s="31">
-        <f t="shared" si="2"/>
+        <f>$L9*F9/F$24</f>
         <v>1</v>
       </c>
       <c r="G18" s="31">
-        <f t="shared" si="2"/>
+        <f>$L9*G9/G$24</f>
         <v>1</v>
       </c>
       <c r="H18" s="31">
-        <f t="shared" si="2"/>
+        <f>$L9*H9/H$24</f>
         <v>0.8</v>
       </c>
       <c r="I18" s="31">
-        <f t="shared" si="2"/>
+        <f>$L9*I9/I$24</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="B19" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="31">
-        <f t="shared" si="1"/>
-        <v>3.7499999999999999E-2</v>
+        <f>$K10*C10/C$24</f>
+        <v>0.0375</v>
       </c>
       <c r="D19" s="31">
-        <f t="shared" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <f>$K10*D10/D$24</f>
+        <v>0.075</v>
       </c>
       <c r="E19" s="31">
-        <f t="shared" si="1"/>
-        <v>7.4999999999999997E-2</v>
+        <f>$K10*E10/E$24</f>
+        <v>0.075</v>
       </c>
       <c r="F19" s="31">
-        <f t="shared" si="2"/>
+        <f>$L10*F10/F$24</f>
         <v>0</v>
       </c>
       <c r="G19" s="31">
-        <f t="shared" si="2"/>
+        <f>$L10*G10/G$24</f>
         <v>0</v>
       </c>
       <c r="H19" s="31">
-        <f t="shared" si="2"/>
+        <f>$L10*H10/H$24</f>
         <v>0</v>
       </c>
       <c r="I19" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+        <f>$L10*I10/I$24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="B20" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="31">
-        <f t="shared" si="1"/>
+        <f>$K11*C11/C$24</f>
         <v>0.15</v>
       </c>
       <c r="D20" s="31">
-        <f t="shared" si="1"/>
+        <f>$K11*D11/D$24</f>
         <v>0.3</v>
       </c>
       <c r="E20" s="31">
-        <f t="shared" si="1"/>
+        <f>$K11*E11/E$24</f>
         <v>0.3</v>
       </c>
       <c r="F20" s="31">
-        <f t="shared" si="2"/>
+        <f>$L11*F11/F$24</f>
         <v>0.2</v>
       </c>
       <c r="G20" s="31">
-        <f t="shared" si="2"/>
-        <v>0.26666666666670003</v>
+        <f>$L11*G11/G$24</f>
+        <v>0.2666666666667</v>
       </c>
       <c r="H20" s="31">
-        <f t="shared" si="2"/>
+        <f>$L11*H11/H$24</f>
         <v>0.08</v>
       </c>
       <c r="I20" s="31">
-        <f t="shared" si="2"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+        <f>$L11*I11/I$24</f>
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="B21" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="31">
-        <f t="shared" si="1"/>
-        <v>1.2500000000000001E-2</v>
+        <f>$K12*C12/C$24</f>
+        <v>0.0125</v>
       </c>
       <c r="D21" s="31">
-        <f t="shared" si="1"/>
-        <v>2.5000000000000001E-2</v>
+        <f>$K12*D12/D$24</f>
+        <v>0.025</v>
       </c>
       <c r="E21" s="31">
-        <f t="shared" si="1"/>
-        <v>2.5000000000000001E-2</v>
+        <f>$K12*E12/E$24</f>
+        <v>0.025</v>
       </c>
       <c r="F21" s="31">
-        <f t="shared" si="2"/>
-        <v>3.3333333333299998E-2</v>
+        <f>$L12*F12/F$24</f>
+        <v>0.0333333333333</v>
       </c>
       <c r="G21" s="31">
-        <f t="shared" si="2"/>
-        <v>3.3333333333299998E-2</v>
+        <f>$L12*G12/G$24</f>
+        <v>0.0333333333333</v>
       </c>
       <c r="H21" s="31">
-        <f t="shared" si="2"/>
+        <f>$L12*H12/H$24</f>
         <v>0.02</v>
       </c>
       <c r="I21" s="31">
-        <f t="shared" si="2"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+        <f>$L12*I12/I$24</f>
+        <v>0.0075</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="B22" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="31">
-        <f t="shared" si="1"/>
+        <f>$K13*C13/C$24</f>
         <v>0.1</v>
       </c>
       <c r="D22" s="31">
-        <f t="shared" si="1"/>
-        <v>0.17499999999999999</v>
+        <f>$K13*D13/D$24</f>
+        <v>0.175</v>
       </c>
       <c r="E22" s="31">
-        <f t="shared" si="1"/>
-        <v>0.17499999999999999</v>
+        <f>$K13*E13/E$24</f>
+        <v>0.175</v>
       </c>
       <c r="F22" s="31">
-        <f t="shared" si="2"/>
-        <v>0.16666666666669999</v>
+        <f>$L13*F13/F$24</f>
+        <v>0.1666666666667</v>
       </c>
       <c r="G22" s="31">
-        <f t="shared" si="2"/>
-        <v>0.16666666666669999</v>
+        <f>$L13*G13/G$24</f>
+        <v>0.1666666666667</v>
       </c>
       <c r="H22" s="31">
-        <f t="shared" si="2"/>
-        <v>0.14000000000000001</v>
+        <f>$L13*H13/H$24</f>
+        <v>0.14</v>
       </c>
       <c r="I22" s="31">
-        <f t="shared" si="2"/>
+        <f>$L13*I13/I$24</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -4516,7 +4506,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
@@ -4550,52 +4540,52 @@
       </c>
       <c r="J24" s="6"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="C26" s="31">
-        <f t="shared" ref="C26:I26" si="3">SUM(C15:C22)</f>
+        <f>SUM(C15:C22)</f>
         <v>2.1</v>
       </c>
       <c r="D26" s="31">
-        <f t="shared" si="3"/>
-        <v>3.4750000000000001</v>
+        <f>SUM(D15:D22)</f>
+        <v>3.475</v>
       </c>
       <c r="E26" s="31">
-        <f t="shared" si="3"/>
-        <v>3.7250000000000001</v>
+        <f>SUM(E15:E22)</f>
+        <v>3.725</v>
       </c>
       <c r="F26" s="31">
-        <f t="shared" si="3"/>
-        <v>4.7333333333332996</v>
+        <f>SUM(F15:F22)</f>
+        <v>4.7333333333333</v>
       </c>
       <c r="G26" s="31">
-        <f t="shared" si="3"/>
-        <v>4.6666666666666998</v>
+        <f>SUM(G15:G22)</f>
+        <v>4.6666666666667</v>
       </c>
       <c r="H26" s="31">
-        <f t="shared" si="3"/>
+        <f>SUM(H15:H22)</f>
         <v>3.32</v>
       </c>
       <c r="I26" s="31">
-        <f t="shared" si="3"/>
-        <v>0.38750000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+        <f>SUM(I15:I22)</f>
+        <v>0.3875</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="C27">
         <f>'cost calculation'!$E11*'Characteristik analyse'!C26</f>
         <v>2.1</v>
       </c>
       <c r="D27" s="6">
         <f>'cost calculation'!$E12*'Characteristik analyse'!D26</f>
-        <v>3.4750000000000001</v>
+        <v>3.475</v>
       </c>
       <c r="E27" s="6">
         <f>'cost calculation'!$E13*'Characteristik analyse'!E26</f>
-        <v>11.175000000000001</v>
+        <v>11.175</v>
       </c>
       <c r="F27" s="6">
         <f>'cost calculation'!$E14*'Characteristik analyse'!F26</f>
-        <v>18.933333333333199</v>
+        <v>18.933333333333</v>
       </c>
       <c r="G27" s="6">
         <f>'cost calculation'!$E15*'Characteristik analyse'!G26</f>
@@ -4611,7 +4601,7 @@
       </c>
       <c r="J27" s="1">
         <f>SUM(C27:I27)</f>
-        <v>35.683333333333195</v>
+        <v>35.683333333333</v>
       </c>
     </row>
   </sheetData>
@@ -4678,7 +4668,7 @@
   <dimension ref="B3:G18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4691,7 +4681,7 @@
     <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
@@ -4711,7 +4701,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="B4" s="7" t="s">
         <v>73</v>
       </c>
@@ -4726,7 +4716,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ref="F4:F17" si="0">E4*D4</f>
+        <f>E4*D4</f>
         <v>6.3</v>
       </c>
       <c r="G4" s="32">
@@ -4734,7 +4724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="B5" s="7" t="s">
         <v>72</v>
       </c>
@@ -4749,7 +4739,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" si="0"/>
+        <f>E5*D5</f>
         <v>0</v>
       </c>
       <c r="G5" s="32">
@@ -4757,22 +4747,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="B6" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="8">
-        <v>8.9499999999999993</v>
+        <v>8.95</v>
       </c>
       <c r="D6" s="8">
         <f>C6/3</f>
-        <v>2.9833333333333329</v>
+        <v>2.9833333333333</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" si="0"/>
+        <f>E6*D6</f>
         <v>0</v>
       </c>
       <c r="G6" s="32">
@@ -4780,12 +4770,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="B7" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C7" s="8">
-        <v>9.4499999999999993</v>
+        <v>9.45</v>
       </c>
       <c r="D7" s="8">
         <f>C7/3</f>
@@ -4795,15 +4785,15 @@
         <v>3</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" si="0"/>
-        <v>9.4499999999999993</v>
+        <f>E7*D7</f>
+        <v>9.45</v>
       </c>
       <c r="G7" s="32">
         <f>Tabelle4[[#This Row],[€ genutzt/Packung]]/Tabelle4[[#This Row],[€/Packung]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="B8" s="7" t="s">
         <v>69</v>
       </c>
@@ -4818,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="0"/>
+        <f>E8*D8</f>
         <v>0</v>
       </c>
       <c r="G8" s="32">
@@ -4826,7 +4816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="B9" s="7" t="s">
         <v>68</v>
       </c>
@@ -4841,7 +4831,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="0"/>
+        <f>E9*D9</f>
         <v>10.36</v>
       </c>
       <c r="G9" s="32">
@@ -4849,22 +4839,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="B10" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="8">
-        <v>35.200000000000003</v>
+        <v>35.2</v>
       </c>
       <c r="D10" s="8">
         <f>C10/20</f>
-        <v>1.7600000000000002</v>
+        <v>1.76</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" si="0"/>
+        <f>E10*D10</f>
         <v>0</v>
       </c>
       <c r="G10" s="32">
@@ -4872,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="B11" s="7" t="s">
         <v>66</v>
       </c>
@@ -4887,7 +4877,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="0"/>
+        <f>E11*D11</f>
         <v>0</v>
       </c>
       <c r="G11" s="32">
@@ -4895,22 +4885,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="B12" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="8">
-        <v>19.989999999999998</v>
+        <v>19.99</v>
       </c>
       <c r="D12" s="8">
         <f>C12/10</f>
-        <v>1.9989999999999999</v>
+        <v>1.999</v>
       </c>
       <c r="E12" s="6">
         <v>0</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="0"/>
+        <f>E12*D12</f>
         <v>0</v>
       </c>
       <c r="G12" s="32">
@@ -4918,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="B13" s="7" t="s">
         <v>64</v>
       </c>
@@ -4933,7 +4923,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="0"/>
+        <f>E13*D13</f>
         <v>0</v>
       </c>
       <c r="G13" s="32">
@@ -4941,22 +4931,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="B14" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="8">
-        <v>19.989999999999998</v>
+        <v>19.99</v>
       </c>
       <c r="D14" s="8">
         <f>C14/3</f>
-        <v>6.6633333333333331</v>
+        <v>6.6633333333333</v>
       </c>
       <c r="E14" s="6">
         <v>0</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="0"/>
+        <f>E14*D14</f>
         <v>0</v>
       </c>
       <c r="G14" s="32">
@@ -4964,7 +4954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="B15" s="7" t="s">
         <v>62</v>
       </c>
@@ -4973,13 +4963,13 @@
       </c>
       <c r="D15" s="8">
         <f>C15/2</f>
-        <v>5.9950000000000001</v>
+        <v>5.995</v>
       </c>
       <c r="E15" s="6">
         <v>0</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="0"/>
+        <f>E15*D15</f>
         <v>0</v>
       </c>
       <c r="G15" s="32">
@@ -4987,22 +4977,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="B16" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="8">
-        <v>19.989999999999998</v>
+        <v>19.99</v>
       </c>
       <c r="D16" s="8">
         <f>C16/20</f>
-        <v>0.99949999999999994</v>
+        <v>0.9995</v>
       </c>
       <c r="E16" s="6">
         <v>0</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="0"/>
+        <f>E16*D16</f>
         <v>0</v>
       </c>
       <c r="G16" s="32">
@@ -5010,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="1" s="6">
       <c r="B17" s="7" t="s">
         <v>74</v>
       </c>
@@ -5019,34 +5009,34 @@
       </c>
       <c r="D17" s="8">
         <f>C17/10</f>
-        <v>2.2749999999999999</v>
+        <v>2.275</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="0"/>
-        <v>2.2749999999999999</v>
+        <f>E17*D17</f>
+        <v>2.275</v>
       </c>
       <c r="G17" s="32">
         <f>Tabelle4[[#This Row],[€ genutzt/Packung]]/Tabelle4[[#This Row],[€/Packung]]</f>
-        <v>9.9999999999999992E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="9">
         <f>SUM(C4:C17)</f>
-        <v>217.15000000000003</v>
+        <v>217.15</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F18" s="9">
         <f>SUM(F4:F17)</f>
-        <v>28.384999999999998</v>
+        <v>28.385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed costs and added some info to the md file.
</commit_message>
<xml_diff>
--- a/kai/kai-warband_orks_mostlyepic_goblins.xlsx
+++ b/kai/kai-warband_orks_mostlyepic_goblins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\Dropbox\Privat\Mordheim\kai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4CDF98-2F92-41F7-A631-6629A3EB9B24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D1D834-02D1-43FE-AF78-76D1C74988F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="warband detail" sheetId="5" r:id="rId1"/>
@@ -854,61 +854,6 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
@@ -1019,6 +964,61 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1033,36 +1033,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="C21:U39" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ausrüstung gesamt"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Typ"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Range"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="S" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="S" dataDxfId="19"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SP"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="gold/stück"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Boss" dataDxfId="25">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Boss" dataDxfId="18">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="schamane" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="big'uns" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="goblin" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="squig" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="boy" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="troll" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="kosten" dataDxfId="18">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="schamane" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="big'uns" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="goblin" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="squig" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="boy" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="troll" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="kosten" dataDxfId="11">
       <calculatedColumnFormula>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="wunsch" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="wunsch" dataDxfId="10">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="zusatzkosten" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="zusatzkosten" dataDxfId="9">
       <calculatedColumnFormula>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gruppe" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Bewertung" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Warband Equip Rating" dataDxfId="13">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gruppe" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Bewertung" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Warband Equip Rating" dataDxfId="6">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1071,17 +1071,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle4" displayName="Tabelle4" ref="B3:G17" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle4" displayName="Tabelle4" ref="B3:G17" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B3:G17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Mögliche einheiten" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="€/Packung" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="€/Figur" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Mögliche einheiten" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="€/Packung" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="€/Figur" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Genutzte figuren"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="€ genutzt/Packung" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="€ genutzt/Packung" dataDxfId="1">
       <calculatedColumnFormula>E4*D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Prozentuale Nutzung" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Prozentuale Nutzung" dataDxfId="0">
       <calculatedColumnFormula>Tabelle4[[#This Row],[€ genutzt/Packung]]/Tabelle4[[#This Row],[€/Packung]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1354,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1998,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD120"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3705,7 +3705,7 @@
     <mergeCell ref="L20:O20"/>
   </mergeCells>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="6" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="55" operator="greaterThan">
       <formula>$C$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3806,32 +3806,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:O22">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I39">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:O39">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:O39">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E17">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed dowuble handed cost as described in mordheim rules.
</commit_message>
<xml_diff>
--- a/kai/kai-warband_orks_mostlyepic_goblins.xlsx
+++ b/kai/kai-warband_orks_mostlyepic_goblins.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\Dropbox\Privat\Mordheim\kai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862B5E6E-D57F-4B16-9936-301B380AC223}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34241CE9-E4B8-4941-A83B-3647238B8AB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cost calculation" sheetId="1" r:id="rId1"/>
-    <sheet name="Characteristik analyse" sheetId="2" r:id="rId2"/>
+    <sheet name="Characteristic analysis" sheetId="2" r:id="rId2"/>
     <sheet name="Boxen" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,47 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="138">
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>axt</t>
-  </si>
-  <si>
-    <t>schwert</t>
-  </si>
-  <si>
-    <t>zweihänder</t>
-  </si>
-  <si>
-    <t>armbrust</t>
-  </si>
-  <si>
-    <t>bogen</t>
-  </si>
-  <si>
-    <t>leichte rüstung</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
   <si>
     <t>helm</t>
   </si>
   <si>
-    <t>schild</t>
-  </si>
-  <si>
-    <t>dolch (+1)</t>
-  </si>
-  <si>
-    <t>speer</t>
-  </si>
-  <si>
     <t>troll</t>
   </si>
   <si>
-    <t>kosten</t>
-  </si>
-  <si>
     <t>anzahl</t>
   </si>
   <si>
@@ -83,18 +50,12 @@
     <t>Warband</t>
   </si>
   <si>
-    <t>verteilt</t>
-  </si>
-  <si>
     <t>Mögliche einheiten</t>
   </si>
   <si>
     <t>gold/einheit</t>
   </si>
   <si>
-    <t>gold/stück</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -122,9 +83,6 @@
     <t>Ld</t>
   </si>
   <si>
-    <t>Boss</t>
-  </si>
-  <si>
     <t>WS/g</t>
   </si>
   <si>
@@ -185,9 +143,6 @@
     <t>Orc Greatax Regiment (Kings of War)</t>
   </si>
   <si>
-    <t>Typ</t>
-  </si>
-  <si>
     <t>cc</t>
   </si>
   <si>
@@ -200,12 +155,6 @@
     <t>30"</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t>24"</t>
   </si>
   <si>
@@ -257,30 +206,12 @@
     <t>€ genutzt/Packung</t>
   </si>
   <si>
-    <t>ausrüstung gesamt</t>
-  </si>
-  <si>
     <t>Prozentuale Nutzung</t>
   </si>
   <si>
-    <t>wunsch</t>
-  </si>
-  <si>
-    <t>zusatzkosten</t>
-  </si>
-  <si>
-    <t>Gruppe</t>
-  </si>
-  <si>
     <t>heros</t>
   </si>
   <si>
-    <t>ork boss (1)</t>
-  </si>
-  <si>
-    <t>schamane (0-1)</t>
-  </si>
-  <si>
     <t>big'uns (0-3)</t>
   </si>
   <si>
@@ -293,9 +224,6 @@
     <t>ork boy</t>
   </si>
   <si>
-    <t>morgenstern</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -311,39 +239,21 @@
     <t>Two-Handed, Last strike</t>
   </si>
   <si>
-    <t>hellebarde</t>
-  </si>
-  <si>
     <t>user+1</t>
   </si>
   <si>
     <t>Two-Handed</t>
   </si>
   <si>
-    <t>wurfwaffen</t>
-  </si>
-  <si>
     <t>Move or Fire</t>
   </si>
   <si>
-    <t>keule</t>
-  </si>
-  <si>
-    <t>kurzbogen</t>
-  </si>
-  <si>
     <t>16"</t>
   </si>
   <si>
-    <t>squig schubser</t>
-  </si>
-  <si>
     <t>12"</t>
   </si>
   <si>
-    <t>ball und kette</t>
-  </si>
-  <si>
     <t>Two-Handed, Incredible, Force, Cumbersome, Unwieldy, Random</t>
   </si>
   <si>
@@ -368,9 +278,6 @@
     <t>Anzahl</t>
   </si>
   <si>
-    <t>schamane</t>
-  </si>
-  <si>
     <t>big'uns</t>
   </si>
   <si>
@@ -395,27 +302,12 @@
     <t>(schlecht) 1 .. 10 (sehr gut)</t>
   </si>
   <si>
-    <t>Bewertung</t>
-  </si>
-  <si>
     <t>Warband Equip Rating</t>
   </si>
   <si>
     <t>Equip rating</t>
   </si>
   <si>
-    <t>Orks (Boss, Bit'Uns)</t>
-  </si>
-  <si>
-    <t>Schamane</t>
-  </si>
-  <si>
-    <t>Goblins</t>
-  </si>
-  <si>
-    <t>v1.6</t>
-  </si>
-  <si>
     <t>er off</t>
   </si>
   <si>
@@ -441,6 +333,117 @@
   </si>
   <si>
     <t>cutting edge enemy armor save -1</t>
+  </si>
+  <si>
+    <t>shield</t>
+  </si>
+  <si>
+    <t>light armor</t>
+  </si>
+  <si>
+    <t>ball and chain</t>
+  </si>
+  <si>
+    <t>squig podder</t>
+  </si>
+  <si>
+    <t>short bow</t>
+  </si>
+  <si>
+    <t>spear</t>
+  </si>
+  <si>
+    <t>club</t>
+  </si>
+  <si>
+    <t>bow</t>
+  </si>
+  <si>
+    <t>crossbow</t>
+  </si>
+  <si>
+    <t>hand weapon</t>
+  </si>
+  <si>
+    <t>helbeard</t>
+  </si>
+  <si>
+    <t>double handed</t>
+  </si>
+  <si>
+    <t>sword</t>
+  </si>
+  <si>
+    <t>morning star</t>
+  </si>
+  <si>
+    <t>battle axe</t>
+  </si>
+  <si>
+    <t>dagger</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>gc/unit</t>
+  </si>
+  <si>
+    <t>leader</t>
+  </si>
+  <si>
+    <t>shaman</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>whish</t>
+  </si>
+  <si>
+    <t>whish cost</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Orks (Leader, Bit'Uns)</t>
+  </si>
+  <si>
+    <t>Shaman</t>
+  </si>
+  <si>
+    <t>Goblins/Orks</t>
+  </si>
+  <si>
+    <t>schaman (0-1)</t>
+  </si>
+  <si>
+    <t>ork boss/leader (1)</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>gold crown</t>
+  </si>
+  <si>
+    <t>v1.7</t>
   </si>
 </sst>
 </file>
@@ -851,34 +854,34 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="C21:U39" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="C21:U39" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ausrüstung gesamt"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Typ"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Range"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="S" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SP"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="gold/stück"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Boss" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="range"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="strength" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="rule"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="gc/unit"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="leader" dataDxfId="18">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="schamane" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="shaman" dataDxfId="17"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="big'uns" dataDxfId="16"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="goblin" dataDxfId="15"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="squig" dataDxfId="14"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="boy" dataDxfId="13"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="troll" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="kosten" dataDxfId="11">
-      <calculatedColumnFormula>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="cost" dataDxfId="11">
+      <calculatedColumnFormula>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="wunsch" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="whish" dataDxfId="10">
       <calculatedColumnFormula>#REF!+#REF!+#REF!+#REF!+#REF!+#REF!+#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="zusatzkosten" dataDxfId="9">
-      <calculatedColumnFormula>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="whish cost" dataDxfId="9">
+      <calculatedColumnFormula>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gruppe" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Bewertung" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="group" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="rating" dataDxfId="7"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Warband Equip Rating" dataDxfId="6">
-      <calculatedColumnFormula>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</calculatedColumnFormula>
+      <calculatedColumnFormula>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1169,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1211,25 +1214,25 @@
   <sheetData>
     <row r="2" spans="2:18" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="22">
-        <v>43340</v>
+        <v>43376</v>
       </c>
     </row>
     <row r="3" spans="2:18" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="21"/>
       <c r="H3" s="6" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="I3" s="1">
         <v>10</v>
@@ -1237,7 +1240,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="H4" s="11" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="I4" s="10">
         <f>5*E18+E11*F11+E12*F12+E13*F13+E14*F14+E15*F15+E16*F16+E17*F17+5</f>
@@ -1246,13 +1249,13 @@
     </row>
     <row r="5" spans="2:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="C5" s="4">
         <v>500</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="I5" s="10">
         <f>ROUNDUP(E18/4,0)</f>
@@ -1261,18 +1264,18 @@
     </row>
     <row r="6" spans="2:18" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C6" s="4">
         <f>G18+P40</f>
         <v>500</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="I6" s="38">
         <f>U40</f>
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="J6" s="6">
         <f>U41</f>
@@ -1280,12 +1283,12 @@
       </c>
       <c r="K6" s="6">
         <f>U42</f>
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C7" s="33">
         <f>C5-C6</f>
@@ -1293,39 +1296,39 @@
       </c>
       <c r="I7" s="2">
         <f>I3+(I6+I4)*I5</f>
-        <v>784</v>
+        <v>805</v>
       </c>
     </row>
     <row r="9" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C10" s="12" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="39" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="D11" s="6">
         <v>80</v>
@@ -1341,16 +1344,16 @@
         <v>80</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="39"/>
       <c r="C12" s="6" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="D12" s="6">
         <v>40</v>
@@ -1366,16 +1369,16 @@
         <v>40</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="39"/>
       <c r="C13" s="6" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D13" s="6">
         <v>40</v>
@@ -1393,10 +1396,10 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="39" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="D14" s="6">
         <v>15</v>
@@ -1415,7 +1418,7 @@
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="39"/>
       <c r="C15" s="6" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D15" s="6">
         <v>15</v>
@@ -1434,7 +1437,7 @@
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="39"/>
       <c r="C16" s="6" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D16" s="6">
         <v>25</v>
@@ -1453,7 +1456,7 @@
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" s="39"/>
       <c r="C17" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D17" s="5">
         <v>200</v>
@@ -1471,7 +1474,7 @@
     </row>
     <row r="18" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="16" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2">
         <f>SUM(E11:E17)</f>
@@ -1487,7 +1490,7 @@
       <c r="B19" s="17"/>
       <c r="F19" s="1"/>
       <c r="I19" s="40" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
@@ -1500,89 +1503,89 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="I20" s="40" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J20" s="40"/>
       <c r="K20" s="40"/>
       <c r="L20" s="40" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="M20" s="40"/>
       <c r="N20" s="40"/>
       <c r="O20" s="40"/>
       <c r="T20" s="6" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="12" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="P21" s="12" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="Q21" s="12" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="R21" s="12" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="S21" s="12" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="U21" s="12" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C22" s="6" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="18" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="H22" s="6">
         <v>2</v>
@@ -1609,37 +1612,37 @@
         <v>0</v>
       </c>
       <c r="P22" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q22" s="6">
         <v>0</v>
       </c>
       <c r="R22" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S22" s="30" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="T22" s="30">
         <v>1</v>
       </c>
       <c r="U22" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="6" t="s">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="6" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="H23" s="6">
         <v>5</v>
@@ -1666,39 +1669,39 @@
         <v>0</v>
       </c>
       <c r="P23" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>10</v>
       </c>
       <c r="Q23" s="6">
         <v>0</v>
       </c>
       <c r="R23" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S23" s="30" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="T23" s="30">
         <v>4</v>
       </c>
       <c r="U23" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C24" s="6" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F24" s="29" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="H24" s="6">
         <v>15</v>
@@ -1725,39 +1728,39 @@
         <v>0</v>
       </c>
       <c r="P24" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q24" s="6">
         <v>0</v>
       </c>
       <c r="R24" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S24" s="30" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="T24" s="30">
         <v>9</v>
       </c>
       <c r="U24" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C25" s="6" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="H25" s="6">
         <v>10</v>
@@ -1784,42 +1787,42 @@
         <v>0</v>
       </c>
       <c r="P25" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>30</v>
       </c>
       <c r="Q25" s="6">
         <v>0</v>
       </c>
       <c r="R25" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S25" s="30" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="T25" s="30">
         <v>5</v>
       </c>
       <c r="U25" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C26" s="6" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="H26" s="6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I26" s="6">
         <v>1</v>
@@ -1843,39 +1846,39 @@
         <v>0</v>
       </c>
       <c r="P26" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>15</v>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
+        <v>10</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
       </c>
       <c r="R26" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S26" s="30" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="T26" s="30">
         <v>8</v>
       </c>
       <c r="U26" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C27" s="6" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="H27" s="6">
         <v>10</v>
@@ -1902,33 +1905,33 @@
         <v>0</v>
       </c>
       <c r="P27" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>10</v>
       </c>
       <c r="Q27" s="6">
         <v>0</v>
       </c>
       <c r="R27" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S27" s="30" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="T27" s="30">
         <v>7</v>
       </c>
       <c r="U27" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C28" s="6" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F28" s="29"/>
       <c r="H28" s="6">
@@ -1956,42 +1959,42 @@
         <v>0</v>
       </c>
       <c r="P28" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q28" s="6">
         <v>0</v>
       </c>
       <c r="R28" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S28" s="30" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="T28" s="30">
         <v>2</v>
       </c>
       <c r="U28" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C29" s="6" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F29" s="29">
         <v>4</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="H29" s="6">
         <v>25</v>
@@ -2018,36 +2021,36 @@
         <v>0</v>
       </c>
       <c r="P29" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q29" s="6">
         <v>0</v>
       </c>
       <c r="R29" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S29" s="30" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="T29" s="30">
         <v>6</v>
       </c>
       <c r="U29" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C30" s="6" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F30" s="29">
         <v>3</v>
@@ -2077,33 +2080,33 @@
         <v>0</v>
       </c>
       <c r="P30" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q30" s="6">
         <v>0</v>
       </c>
       <c r="R30" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S30" s="30" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="T30" s="30">
         <v>6</v>
       </c>
       <c r="U30" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C31" s="6" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F31" s="29"/>
       <c r="H31" s="6">
@@ -2131,39 +2134,39 @@
         <v>0</v>
       </c>
       <c r="P31" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q31" s="6">
         <v>0</v>
       </c>
       <c r="R31" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S31" s="30" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="T31" s="30">
         <v>2</v>
       </c>
       <c r="U31" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C32" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F32" s="29" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="H32" s="6">
         <v>5</v>
@@ -2190,36 +2193,36 @@
         <v>0</v>
       </c>
       <c r="P32" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>15</v>
       </c>
       <c r="Q32" s="6">
         <v>0</v>
       </c>
       <c r="R32" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="T32" s="30">
         <v>5</v>
       </c>
       <c r="U32" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C33" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="F33" s="29">
         <v>3</v>
@@ -2249,36 +2252,36 @@
         <v>0</v>
       </c>
       <c r="P33" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>20</v>
       </c>
       <c r="Q33" s="6">
         <v>0</v>
       </c>
       <c r="R33" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S33" s="30" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="T33" s="30">
         <v>5</v>
       </c>
       <c r="U33" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C34" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="F34" s="29"/>
       <c r="H34" s="6">
@@ -2306,24 +2309,24 @@
         <v>0</v>
       </c>
       <c r="P34" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q34" s="6">
         <v>0</v>
       </c>
       <c r="R34" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S34" s="30" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="T34" s="30">
         <v>3</v>
       </c>
       <c r="U34" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
@@ -2332,13 +2335,13 @@
         <v>104</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H35" s="6">
         <v>15</v>
@@ -2365,33 +2368,33 @@
         <v>0</v>
       </c>
       <c r="P35" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q35" s="6">
         <v>0</v>
       </c>
       <c r="R35" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S35" s="30" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="T35" s="30">
         <v>9</v>
       </c>
       <c r="U35" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C36" s="34" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E36" s="34"/>
       <c r="F36" s="35"/>
@@ -2421,37 +2424,37 @@
         <v>0</v>
       </c>
       <c r="P36" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q36" s="6">
         <v>0</v>
       </c>
       <c r="R36" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S36" s="30" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="T36" s="30">
         <v>5</v>
       </c>
       <c r="U36" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C37" s="6" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F37" s="29"/>
       <c r="G37" s="6" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="H37" s="6">
         <v>20</v>
@@ -2478,38 +2481,38 @@
         <v>0</v>
       </c>
       <c r="P37" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>80</v>
       </c>
       <c r="Q37" s="6">
         <v>0</v>
       </c>
       <c r="R37" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S37" s="30" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="T37" s="30">
         <v>8</v>
       </c>
       <c r="U37" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>32</v>
       </c>
     </row>
     <row r="38" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C38" s="6" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E38" s="34"/>
       <c r="F38" s="35"/>
       <c r="G38" s="34" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="H38" s="6">
         <v>5</v>
@@ -2521,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="6">
         <v>3</v>
@@ -2536,38 +2539,38 @@
         <v>0</v>
       </c>
       <c r="P38" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
-        <v>20</v>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
+        <v>25</v>
       </c>
       <c r="Q38" s="6">
         <v>0</v>
       </c>
       <c r="R38" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S38" s="30" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="T38" s="30">
         <v>7</v>
       </c>
       <c r="U38" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
-        <v>28</v>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C39" s="34" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E39" s="34"/>
       <c r="F39" s="35"/>
       <c r="G39" s="34" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="H39" s="34">
         <v>10</v>
@@ -2594,24 +2597,24 @@
         <v>0</v>
       </c>
       <c r="P39" s="6">
-        <f>SUM(Tabelle2[[#This Row],[Boss]:[troll]])*Tabelle2[[#This Row],[gold/stück]]</f>
+        <f>SUM(Tabelle2[[#This Row],[leader]:[troll]])*Tabelle2[[#This Row],[gc/unit]]</f>
         <v>0</v>
       </c>
       <c r="Q39" s="6">
         <v>0</v>
       </c>
       <c r="R39" s="6">
-        <f>Tabelle2[[#This Row],[gold/stück]]*Tabelle2[[#This Row],[wunsch]]</f>
+        <f>Tabelle2[[#This Row],[gc/unit]]*Tabelle2[[#This Row],[whish]]</f>
         <v>0</v>
       </c>
       <c r="S39" s="30" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="T39" s="30">
         <v>7</v>
       </c>
       <c r="U39" s="30">
-        <f>Tabelle2[[#This Row],[Bewertung]]*SUM(Tabelle2[[#This Row],[Boss]:[troll]])</f>
+        <f>Tabelle2[[#This Row],[rating]]*SUM(Tabelle2[[#This Row],[leader]:[troll]])</f>
         <v>0</v>
       </c>
     </row>
@@ -2624,7 +2627,7 @@
       <c r="H40" s="34"/>
       <c r="I40" s="3">
         <f t="shared" ref="I40:O40" si="1">I22*$H22+I23*$H23+I24*$H24+I25*$H25+I26*$H26+I27*$H27+I28*$H28+I29*$H29+I30*$H30+I31*$H31+I32*$H32+I33*$H33+I34*$H34+I35*$H35+I36*$H36+I37*$H37+I38*$H38+I39*$H39</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J40" s="3">
         <f t="shared" si="1"/>
@@ -2632,7 +2635,7 @@
       </c>
       <c r="K40" s="3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="L40" s="3">
         <f t="shared" si="1"/>
@@ -2656,23 +2659,23 @@
       </c>
       <c r="Q40" s="34"/>
       <c r="R40" s="37">
-        <f>SUM(Tabelle2[zusatzkosten])</f>
+        <f>SUM(Tabelle2[whish cost])</f>
         <v>0</v>
       </c>
       <c r="S40" s="36"/>
       <c r="T40" s="6" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="U40" s="2">
         <f>SUM(Tabelle2[Warband Equip Rating])</f>
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F41" s="29"/>
       <c r="S41" s="30"/>
       <c r="T41" s="6" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="U41" s="6">
         <f>SUM(U22:U36)</f>
@@ -2683,11 +2686,11 @@
       <c r="F42" s="29"/>
       <c r="S42" s="30"/>
       <c r="T42" s="6" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="U42" s="6">
         <f>SUM(U37:U39)</f>
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="3:21" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3031,7 +3034,7 @@
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3051,18 +3054,18 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" s="41" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
@@ -3071,11 +3074,11 @@
       <c r="B4" s="13"/>
       <c r="C4" s="12" t="str">
         <f>'cost calculation'!C11</f>
-        <v>ork boss (1)</v>
+        <v>ork boss/leader (1)</v>
       </c>
       <c r="D4" s="12" t="str">
         <f>'cost calculation'!C12</f>
-        <v>schamane (0-1)</v>
+        <v>schaman (0-1)</v>
       </c>
       <c r="E4" s="12" t="str">
         <f>'cost calculation'!C13</f>
@@ -3098,13 +3101,13 @@
         <v>troll</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="L4" s="40"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3128,15 +3131,15 @@
         <v>6</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -3169,7 +3172,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -3202,7 +3205,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3235,7 +3238,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -3268,7 +3271,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3301,7 +3304,7 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -3334,7 +3337,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3366,7 +3369,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="14" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -3408,7 +3411,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="15" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C15" s="31">
         <f t="shared" ref="C15:E22" si="1">$K6*C6/C$24</f>
@@ -3441,7 +3444,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C16" s="31">
         <f t="shared" si="1"/>
@@ -3474,7 +3477,7 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C17" s="31">
         <f t="shared" si="1"/>
@@ -3507,7 +3510,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="15" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C18" s="31">
         <f t="shared" si="1"/>
@@ -3540,7 +3543,7 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="15" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C19" s="31">
         <f t="shared" si="1"/>
@@ -3573,7 +3576,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="15" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C20" s="31">
         <f t="shared" si="1"/>
@@ -3606,7 +3609,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C21" s="31">
         <f t="shared" si="1"/>
@@ -3639,7 +3642,7 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C22" s="31">
         <f t="shared" si="1"/>
@@ -3683,7 +3686,7 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="16" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C24" s="11">
         <f>'cost calculation'!D11</f>
@@ -3747,31 +3750,31 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C27">
-        <f>'cost calculation'!$E11*'Characteristik analyse'!C26</f>
+        <f>'cost calculation'!$E11*'Characteristic analysis'!C26</f>
         <v>2.1</v>
       </c>
       <c r="D27" s="6">
-        <f>'cost calculation'!$E12*'Characteristik analyse'!D26</f>
+        <f>'cost calculation'!$E12*'Characteristic analysis'!D26</f>
         <v>3.4750000000000001</v>
       </c>
       <c r="E27" s="6">
-        <f>'cost calculation'!$E13*'Characteristik analyse'!E26</f>
+        <f>'cost calculation'!$E13*'Characteristic analysis'!E26</f>
         <v>11.175000000000001</v>
       </c>
       <c r="F27" s="6">
-        <f>'cost calculation'!$E14*'Characteristik analyse'!F26</f>
+        <f>'cost calculation'!$E14*'Characteristic analysis'!F26</f>
         <v>18.933333333333</v>
       </c>
       <c r="G27" s="6">
-        <f>'cost calculation'!$E15*'Characteristik analyse'!G26</f>
+        <f>'cost calculation'!$E15*'Characteristic analysis'!G26</f>
         <v>0</v>
       </c>
       <c r="H27" s="6">
-        <f>'cost calculation'!$E16*'Characteristik analyse'!H26</f>
+        <f>'cost calculation'!$E16*'Characteristic analysis'!H26</f>
         <v>0</v>
       </c>
       <c r="I27" s="6">
-        <f>'cost calculation'!$E17*'Characteristik analyse'!I26</f>
+        <f>'cost calculation'!$E17*'Characteristic analysis'!I26</f>
         <v>0</v>
       </c>
       <c r="J27" s="1">
@@ -3858,27 +3861,27 @@
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8">
         <v>6.3</v>
@@ -3901,7 +3904,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C5" s="8">
         <v>10.71</v>
@@ -3924,7 +3927,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C6" s="8">
         <v>8.9499999999999993</v>
@@ -3947,7 +3950,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C7" s="8">
         <v>9.4499999999999993</v>
@@ -3970,7 +3973,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C8" s="8">
         <v>11.99</v>
@@ -3993,7 +3996,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C9" s="8">
         <v>10.36</v>
@@ -4016,7 +4019,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C10" s="8">
         <v>35.200000000000003</v>
@@ -4039,7 +4042,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C11" s="8">
         <v>21.49</v>
@@ -4062,7 +4065,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C12" s="8">
         <v>19.989999999999998</v>
@@ -4085,7 +4088,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C13" s="8">
         <v>7.99</v>
@@ -4108,7 +4111,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C14" s="8">
         <v>19.989999999999998</v>
@@ -4131,7 +4134,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C15" s="8">
         <v>11.99</v>
@@ -4154,7 +4157,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C16" s="8">
         <v>19.989999999999998</v>
@@ -4177,7 +4180,7 @@
     </row>
     <row r="17" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C17" s="8">
         <v>22.75</v>
@@ -4200,14 +4203,14 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C18" s="9">
         <f>SUM(C4:C17)</f>
         <v>217.15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F18" s="9">
         <f>SUM(F4:F17)</f>

</xml_diff>